<commit_message>
refactor: all structure was refactored
</commit_message>
<xml_diff>
--- a/exports/model.xlsx
+++ b/exports/model.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabiomantelli/Documents/Repositories/medfasee/stat-python/exports/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002475BB-D336-E742-B30C-FC2F329F7315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="570" windowWidth="28455" windowHeight="11955"/>
+    <workbookView xWindow="240" yWindow="740" windowWidth="28460" windowHeight="11960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Síntese" sheetId="1" r:id="rId1"/>
+    <sheet name="Sintese" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -126,11 +132,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hh:mm:ss.000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,17 +147,20 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -196,7 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -261,32 +270,40 @@
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle name="Síntese-style" pivot="0" count="3">
+    <tableStyle name="Síntese-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="B2:O228" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="B2:O228" headerRowCount="0">
   <tableColumns count="14">
-    <tableColumn id="1" name="Column1"/>
-    <tableColumn id="2" name="Column2"/>
-    <tableColumn id="3" name="Column3"/>
-    <tableColumn id="4" name="Column4"/>
-    <tableColumn id="5" name="Column5"/>
-    <tableColumn id="6" name="Column6"/>
-    <tableColumn id="7" name="Column7"/>
-    <tableColumn id="8" name="Column8"/>
-    <tableColumn id="9" name="Column9"/>
-    <tableColumn id="10" name="Column10"/>
-    <tableColumn id="11" name="Column11"/>
-    <tableColumn id="12" name="Column12"/>
-    <tableColumn id="13" name="Column13"/>
-    <tableColumn id="14" name="Column14"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Column9"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column10"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column11"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Column12"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Column13"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Column14"/>
   </tableColumns>
   <tableStyleInfo name="Síntese-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -494,34 +511,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="2.5" customWidth="1"/>
+    <col min="2" max="2" width="5.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" customWidth="1"/>
-    <col min="16" max="27" width="8.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.5" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" customWidth="1"/>
+    <col min="13" max="13" width="19.5" customWidth="1"/>
+    <col min="14" max="14" width="15.5" customWidth="1"/>
+    <col min="15" max="15" width="16.83203125" customWidth="1"/>
+    <col min="16" max="27" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="12" customHeight="1">
+    <row r="1" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="1"/>
@@ -549,7 +566,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" ht="25.5" customHeight="1">
+    <row r="2" spans="1:27" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -606,7 +623,7 @@
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="7">
         <v>2</v>
@@ -663,7 +680,7 @@
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:27" ht="15" customHeight="1">
+    <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="7">
         <v>3</v>
@@ -720,7 +737,7 @@
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
     </row>
-    <row r="5" spans="1:27" ht="15" customHeight="1">
+    <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="7">
         <v>4</v>
@@ -777,7 +794,7 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
     </row>
-    <row r="6" spans="1:27" ht="15" customHeight="1">
+    <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="7">
         <v>5</v>
@@ -834,7 +851,7 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
     </row>
-    <row r="7" spans="1:27" ht="15" customHeight="1">
+    <row r="7" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="7">
         <v>6</v>
@@ -891,7 +908,7 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
     </row>
-    <row r="8" spans="1:27" ht="15" customHeight="1">
+    <row r="8" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="7">
         <v>7</v>
@@ -948,7 +965,7 @@
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
     </row>
-    <row r="9" spans="1:27" ht="15" customHeight="1">
+    <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="7">
         <v>8</v>
@@ -1005,7 +1022,7 @@
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
     </row>
-    <row r="10" spans="1:27" ht="15" customHeight="1">
+    <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="7">
         <v>9</v>
@@ -1062,7 +1079,7 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" spans="1:27" ht="15" customHeight="1">
+    <row r="11" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="7">
         <v>10</v>
@@ -1119,7 +1136,7 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="1:27" ht="15" customHeight="1">
+    <row r="12" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="7">
         <v>11</v>
@@ -1176,7 +1193,7 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
     </row>
-    <row r="13" spans="1:27" ht="15" customHeight="1">
+    <row r="13" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="7">
         <v>12</v>
@@ -1233,7 +1250,7 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" spans="1:27" ht="15" customHeight="1">
+    <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="7">
         <v>13</v>
@@ -1290,7 +1307,7 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="1:27" ht="15" customHeight="1">
+    <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="7">
         <v>14</v>
@@ -1347,7 +1364,7 @@
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" spans="1:27" ht="15" customHeight="1">
+    <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="7">
         <v>15</v>
@@ -1404,7 +1421,7 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
     </row>
-    <row r="17" spans="1:27" ht="15" customHeight="1">
+    <row r="17" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="7">
         <v>16</v>
@@ -1459,7 +1476,7 @@
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
     </row>
-    <row r="18" spans="1:27" ht="15" customHeight="1">
+    <row r="18" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="7">
         <v>17</v>
@@ -1514,7 +1531,7 @@
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
     </row>
-    <row r="19" spans="1:27" ht="15" customHeight="1">
+    <row r="19" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="7">
         <v>18</v>
       </c>
@@ -1558,7 +1575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="15" customHeight="1">
+    <row r="20" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="7">
         <v>19</v>
       </c>
@@ -1602,7 +1619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="15" customHeight="1">
+    <row r="21" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="7">
         <v>20</v>
       </c>
@@ -1646,7 +1663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="15" customHeight="1">
+    <row r="22" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="7">
         <v>21</v>
       </c>
@@ -1690,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:27" ht="15" customHeight="1">
+    <row r="23" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="7">
         <v>22</v>
       </c>
@@ -1734,7 +1751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="15" customHeight="1">
+    <row r="24" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="7">
         <v>23</v>
       </c>
@@ -1778,7 +1795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="15" customHeight="1">
+    <row r="25" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="7">
         <v>24</v>
       </c>
@@ -1822,7 +1839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="15" customHeight="1">
+    <row r="26" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="7">
         <v>26</v>
       </c>
@@ -1866,7 +1883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="15" customHeight="1">
+    <row r="27" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="7">
         <v>27</v>
       </c>
@@ -1910,7 +1927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="15" customHeight="1">
+    <row r="28" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="7">
         <v>29</v>
       </c>
@@ -1954,7 +1971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="15.75" customHeight="1">
+    <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="9"/>
       <c r="C29" s="10"/>
       <c r="D29" s="9"/>
@@ -1964,7 +1981,7 @@
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
     </row>
-    <row r="30" spans="1:27" ht="15.75" customHeight="1">
+    <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="9"/>
       <c r="C30" s="10"/>
       <c r="D30" s="9"/>
@@ -1974,7 +1991,7 @@
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
     </row>
-    <row r="31" spans="1:27" ht="15.75" customHeight="1">
+    <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="9"/>
       <c r="C31" s="10"/>
       <c r="D31" s="9"/>
@@ -1984,7 +2001,7 @@
       <c r="H31" s="11"/>
       <c r="I31" s="11"/>
     </row>
-    <row r="32" spans="1:27" ht="15.75" customHeight="1">
+    <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="9"/>
       <c r="C32" s="10"/>
       <c r="D32" s="9"/>
@@ -1994,7 +2011,7 @@
       <c r="H32" s="11"/>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="2:9" ht="15.75" customHeight="1">
+    <row r="33" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="9"/>
       <c r="C33" s="10"/>
       <c r="D33" s="9"/>
@@ -2004,7 +2021,7 @@
       <c r="H33" s="11"/>
       <c r="I33" s="11"/>
     </row>
-    <row r="34" spans="2:9" ht="15.75" customHeight="1">
+    <row r="34" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="9"/>
       <c r="C34" s="10"/>
       <c r="D34" s="9"/>
@@ -2014,7 +2031,7 @@
       <c r="H34" s="11"/>
       <c r="I34" s="11"/>
     </row>
-    <row r="35" spans="2:9" ht="15.75" customHeight="1">
+    <row r="35" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="9"/>
       <c r="C35" s="10"/>
       <c r="D35" s="9"/>
@@ -2024,7 +2041,7 @@
       <c r="H35" s="11"/>
       <c r="I35" s="11"/>
     </row>
-    <row r="36" spans="2:9" ht="15.75" customHeight="1">
+    <row r="36" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="9"/>
       <c r="C36" s="10"/>
       <c r="D36" s="9"/>
@@ -2034,7 +2051,7 @@
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
     </row>
-    <row r="37" spans="2:9" ht="15.75" customHeight="1">
+    <row r="37" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="9"/>
       <c r="C37" s="10"/>
       <c r="D37" s="9"/>
@@ -2044,7 +2061,7 @@
       <c r="H37" s="11"/>
       <c r="I37" s="11"/>
     </row>
-    <row r="38" spans="2:9" ht="15.75" customHeight="1">
+    <row r="38" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="9"/>
       <c r="C38" s="10"/>
       <c r="D38" s="9"/>
@@ -2054,7 +2071,7 @@
       <c r="H38" s="11"/>
       <c r="I38" s="11"/>
     </row>
-    <row r="39" spans="2:9" ht="15.75" customHeight="1">
+    <row r="39" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="9"/>
       <c r="C39" s="10"/>
       <c r="D39" s="9"/>
@@ -2064,7 +2081,7 @@
       <c r="H39" s="11"/>
       <c r="I39" s="11"/>
     </row>
-    <row r="40" spans="2:9" ht="15.75" customHeight="1">
+    <row r="40" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="9"/>
       <c r="C40" s="10"/>
       <c r="D40" s="9"/>
@@ -2074,7 +2091,7 @@
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
     </row>
-    <row r="41" spans="2:9" ht="15.75" customHeight="1">
+    <row r="41" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="9"/>
       <c r="C41" s="10"/>
       <c r="D41" s="9"/>
@@ -2084,7 +2101,7 @@
       <c r="H41" s="11"/>
       <c r="I41" s="11"/>
     </row>
-    <row r="42" spans="2:9" ht="15.75" customHeight="1">
+    <row r="42" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="9"/>
       <c r="C42" s="10"/>
       <c r="D42" s="9"/>
@@ -2094,7 +2111,7 @@
       <c r="H42" s="11"/>
       <c r="I42" s="11"/>
     </row>
-    <row r="43" spans="2:9" ht="15.75" customHeight="1">
+    <row r="43" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="9"/>
       <c r="C43" s="10"/>
       <c r="D43" s="9"/>
@@ -2104,7 +2121,7 @@
       <c r="H43" s="11"/>
       <c r="I43" s="11"/>
     </row>
-    <row r="44" spans="2:9" ht="15.75" customHeight="1">
+    <row r="44" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="9"/>
       <c r="C44" s="10"/>
       <c r="D44" s="9"/>
@@ -2114,7 +2131,7 @@
       <c r="H44" s="11"/>
       <c r="I44" s="11"/>
     </row>
-    <row r="45" spans="2:9" ht="15.75" customHeight="1">
+    <row r="45" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="9"/>
       <c r="C45" s="10"/>
       <c r="D45" s="9"/>
@@ -2124,7 +2141,7 @@
       <c r="H45" s="11"/>
       <c r="I45" s="11"/>
     </row>
-    <row r="46" spans="2:9" ht="15.75" customHeight="1">
+    <row r="46" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="9"/>
       <c r="C46" s="10"/>
       <c r="D46" s="9"/>
@@ -2134,7 +2151,7 @@
       <c r="H46" s="11"/>
       <c r="I46" s="11"/>
     </row>
-    <row r="47" spans="2:9" ht="15.75" customHeight="1">
+    <row r="47" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="9"/>
       <c r="C47" s="10"/>
       <c r="D47" s="9"/>
@@ -2144,7 +2161,7 @@
       <c r="H47" s="11"/>
       <c r="I47" s="11"/>
     </row>
-    <row r="48" spans="2:9" ht="15.75" customHeight="1">
+    <row r="48" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="9"/>
       <c r="C48" s="10"/>
       <c r="D48" s="9"/>
@@ -2154,7 +2171,7 @@
       <c r="H48" s="11"/>
       <c r="I48" s="11"/>
     </row>
-    <row r="49" spans="2:9" ht="15.75" customHeight="1">
+    <row r="49" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="9"/>
       <c r="C49" s="10"/>
       <c r="D49" s="9"/>
@@ -2164,7 +2181,7 @@
       <c r="H49" s="11"/>
       <c r="I49" s="11"/>
     </row>
-    <row r="50" spans="2:9" ht="15.75" customHeight="1">
+    <row r="50" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="9"/>
       <c r="C50" s="10"/>
       <c r="D50" s="9"/>
@@ -2174,7 +2191,7 @@
       <c r="H50" s="11"/>
       <c r="I50" s="11"/>
     </row>
-    <row r="51" spans="2:9" ht="15.75" customHeight="1">
+    <row r="51" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="9"/>
       <c r="C51" s="10"/>
       <c r="D51" s="9"/>
@@ -2184,7 +2201,7 @@
       <c r="H51" s="11"/>
       <c r="I51" s="11"/>
     </row>
-    <row r="52" spans="2:9" ht="15.75" customHeight="1">
+    <row r="52" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="9"/>
       <c r="C52" s="10"/>
       <c r="D52" s="9"/>
@@ -2194,7 +2211,7 @@
       <c r="H52" s="11"/>
       <c r="I52" s="11"/>
     </row>
-    <row r="53" spans="2:9" ht="15.75" customHeight="1">
+    <row r="53" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="9"/>
       <c r="C53" s="10"/>
       <c r="D53" s="9"/>
@@ -2204,7 +2221,7 @@
       <c r="H53" s="11"/>
       <c r="I53" s="11"/>
     </row>
-    <row r="54" spans="2:9" ht="15.75" customHeight="1">
+    <row r="54" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="9"/>
       <c r="C54" s="10"/>
       <c r="D54" s="9"/>
@@ -2214,7 +2231,7 @@
       <c r="H54" s="11"/>
       <c r="I54" s="11"/>
     </row>
-    <row r="55" spans="2:9" ht="15.75" customHeight="1">
+    <row r="55" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="9"/>
       <c r="C55" s="10"/>
       <c r="D55" s="9"/>
@@ -2224,7 +2241,7 @@
       <c r="H55" s="11"/>
       <c r="I55" s="11"/>
     </row>
-    <row r="56" spans="2:9" ht="15.75" customHeight="1">
+    <row r="56" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="9"/>
       <c r="C56" s="10"/>
       <c r="D56" s="9"/>
@@ -2234,7 +2251,7 @@
       <c r="H56" s="11"/>
       <c r="I56" s="11"/>
     </row>
-    <row r="57" spans="2:9" ht="15.75" customHeight="1">
+    <row r="57" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="9"/>
       <c r="C57" s="10"/>
       <c r="D57" s="9"/>
@@ -2244,7 +2261,7 @@
       <c r="H57" s="11"/>
       <c r="I57" s="11"/>
     </row>
-    <row r="58" spans="2:9" ht="15.75" customHeight="1">
+    <row r="58" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="9"/>
       <c r="C58" s="10"/>
       <c r="D58" s="9"/>
@@ -2254,7 +2271,7 @@
       <c r="H58" s="11"/>
       <c r="I58" s="11"/>
     </row>
-    <row r="59" spans="2:9" ht="15.75" customHeight="1">
+    <row r="59" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="9"/>
       <c r="C59" s="10"/>
       <c r="D59" s="9"/>
@@ -2264,7 +2281,7 @@
       <c r="H59" s="11"/>
       <c r="I59" s="11"/>
     </row>
-    <row r="60" spans="2:9" ht="15.75" customHeight="1">
+    <row r="60" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="9"/>
       <c r="C60" s="10"/>
       <c r="D60" s="9"/>
@@ -2274,7 +2291,7 @@
       <c r="H60" s="11"/>
       <c r="I60" s="11"/>
     </row>
-    <row r="61" spans="2:9" ht="15.75" customHeight="1">
+    <row r="61" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="9"/>
       <c r="C61" s="10"/>
       <c r="D61" s="9"/>
@@ -2284,7 +2301,7 @@
       <c r="H61" s="11"/>
       <c r="I61" s="11"/>
     </row>
-    <row r="62" spans="2:9" ht="15.75" customHeight="1">
+    <row r="62" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="9"/>
       <c r="C62" s="10"/>
       <c r="D62" s="9"/>
@@ -2294,7 +2311,7 @@
       <c r="H62" s="11"/>
       <c r="I62" s="11"/>
     </row>
-    <row r="63" spans="2:9" ht="15.75" customHeight="1">
+    <row r="63" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="9"/>
       <c r="C63" s="10"/>
       <c r="D63" s="9"/>
@@ -2304,7 +2321,7 @@
       <c r="H63" s="11"/>
       <c r="I63" s="11"/>
     </row>
-    <row r="64" spans="2:9" ht="15.75" customHeight="1">
+    <row r="64" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="9"/>
       <c r="C64" s="10"/>
       <c r="D64" s="9"/>
@@ -2314,7 +2331,7 @@
       <c r="H64" s="11"/>
       <c r="I64" s="11"/>
     </row>
-    <row r="65" spans="2:9" ht="15.75" customHeight="1">
+    <row r="65" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="9"/>
       <c r="C65" s="10"/>
       <c r="D65" s="9"/>
@@ -2324,7 +2341,7 @@
       <c r="H65" s="11"/>
       <c r="I65" s="11"/>
     </row>
-    <row r="66" spans="2:9" ht="15.75" customHeight="1">
+    <row r="66" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="9"/>
       <c r="C66" s="10"/>
       <c r="D66" s="9"/>
@@ -2334,7 +2351,7 @@
       <c r="H66" s="11"/>
       <c r="I66" s="11"/>
     </row>
-    <row r="67" spans="2:9" ht="15.75" customHeight="1">
+    <row r="67" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="9"/>
       <c r="C67" s="10"/>
       <c r="D67" s="9"/>
@@ -2344,7 +2361,7 @@
       <c r="H67" s="11"/>
       <c r="I67" s="11"/>
     </row>
-    <row r="68" spans="2:9" ht="15.75" customHeight="1">
+    <row r="68" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="9"/>
       <c r="C68" s="10"/>
       <c r="D68" s="9"/>
@@ -2354,7 +2371,7 @@
       <c r="H68" s="11"/>
       <c r="I68" s="11"/>
     </row>
-    <row r="69" spans="2:9" ht="15.75" customHeight="1">
+    <row r="69" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="9"/>
       <c r="C69" s="10"/>
       <c r="D69" s="9"/>
@@ -2364,7 +2381,7 @@
       <c r="H69" s="11"/>
       <c r="I69" s="11"/>
     </row>
-    <row r="70" spans="2:9" ht="15.75" customHeight="1">
+    <row r="70" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B70" s="9"/>
       <c r="C70" s="10"/>
       <c r="D70" s="9"/>
@@ -2374,7 +2391,7 @@
       <c r="H70" s="11"/>
       <c r="I70" s="11"/>
     </row>
-    <row r="71" spans="2:9" ht="15.75" customHeight="1">
+    <row r="71" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="9"/>
       <c r="C71" s="10"/>
       <c r="D71" s="9"/>
@@ -2384,7 +2401,7 @@
       <c r="H71" s="11"/>
       <c r="I71" s="11"/>
     </row>
-    <row r="72" spans="2:9" ht="15.75" customHeight="1">
+    <row r="72" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="9"/>
       <c r="C72" s="10"/>
       <c r="D72" s="9"/>
@@ -2394,7 +2411,7 @@
       <c r="H72" s="11"/>
       <c r="I72" s="11"/>
     </row>
-    <row r="73" spans="2:9" ht="15.75" customHeight="1">
+    <row r="73" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="9"/>
       <c r="C73" s="10"/>
       <c r="D73" s="9"/>
@@ -2404,7 +2421,7 @@
       <c r="H73" s="11"/>
       <c r="I73" s="11"/>
     </row>
-    <row r="74" spans="2:9" ht="15.75" customHeight="1">
+    <row r="74" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="9"/>
       <c r="C74" s="10"/>
       <c r="D74" s="9"/>
@@ -2414,7 +2431,7 @@
       <c r="H74" s="11"/>
       <c r="I74" s="11"/>
     </row>
-    <row r="75" spans="2:9" ht="15.75" customHeight="1">
+    <row r="75" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B75" s="9"/>
       <c r="C75" s="10"/>
       <c r="D75" s="9"/>
@@ -2424,7 +2441,7 @@
       <c r="H75" s="11"/>
       <c r="I75" s="11"/>
     </row>
-    <row r="76" spans="2:9" ht="15.75" customHeight="1">
+    <row r="76" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="9"/>
       <c r="C76" s="10"/>
       <c r="D76" s="9"/>
@@ -2434,7 +2451,7 @@
       <c r="H76" s="11"/>
       <c r="I76" s="11"/>
     </row>
-    <row r="77" spans="2:9" ht="15.75" customHeight="1">
+    <row r="77" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B77" s="9"/>
       <c r="C77" s="10"/>
       <c r="D77" s="9"/>
@@ -2444,7 +2461,7 @@
       <c r="H77" s="11"/>
       <c r="I77" s="11"/>
     </row>
-    <row r="78" spans="2:9" ht="15.75" customHeight="1">
+    <row r="78" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B78" s="9"/>
       <c r="C78" s="10"/>
       <c r="D78" s="9"/>
@@ -2454,7 +2471,7 @@
       <c r="H78" s="11"/>
       <c r="I78" s="11"/>
     </row>
-    <row r="79" spans="2:9" ht="15.75" customHeight="1">
+    <row r="79" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="9"/>
       <c r="C79" s="10"/>
       <c r="D79" s="9"/>
@@ -2464,7 +2481,7 @@
       <c r="H79" s="11"/>
       <c r="I79" s="11"/>
     </row>
-    <row r="80" spans="2:9" ht="15.75" customHeight="1">
+    <row r="80" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B80" s="9"/>
       <c r="C80" s="10"/>
       <c r="D80" s="9"/>
@@ -2474,7 +2491,7 @@
       <c r="H80" s="11"/>
       <c r="I80" s="11"/>
     </row>
-    <row r="81" spans="2:9" ht="15.75" customHeight="1">
+    <row r="81" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B81" s="9"/>
       <c r="C81" s="10"/>
       <c r="D81" s="9"/>
@@ -2484,7 +2501,7 @@
       <c r="H81" s="11"/>
       <c r="I81" s="11"/>
     </row>
-    <row r="82" spans="2:9" ht="15.75" customHeight="1">
+    <row r="82" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="9"/>
       <c r="C82" s="10"/>
       <c r="D82" s="9"/>
@@ -2494,7 +2511,7 @@
       <c r="H82" s="11"/>
       <c r="I82" s="11"/>
     </row>
-    <row r="83" spans="2:9" ht="15.75" customHeight="1">
+    <row r="83" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B83" s="9"/>
       <c r="C83" s="10"/>
       <c r="D83" s="9"/>
@@ -2504,7 +2521,7 @@
       <c r="H83" s="11"/>
       <c r="I83" s="11"/>
     </row>
-    <row r="84" spans="2:9" ht="15.75" customHeight="1">
+    <row r="84" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B84" s="9"/>
       <c r="C84" s="10"/>
       <c r="D84" s="9"/>
@@ -2514,7 +2531,7 @@
       <c r="H84" s="11"/>
       <c r="I84" s="11"/>
     </row>
-    <row r="85" spans="2:9" ht="15.75" customHeight="1">
+    <row r="85" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B85" s="9"/>
       <c r="C85" s="10"/>
       <c r="D85" s="9"/>
@@ -2524,7 +2541,7 @@
       <c r="H85" s="11"/>
       <c r="I85" s="11"/>
     </row>
-    <row r="86" spans="2:9" ht="15.75" customHeight="1">
+    <row r="86" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B86" s="9"/>
       <c r="C86" s="10"/>
       <c r="D86" s="9"/>
@@ -2534,7 +2551,7 @@
       <c r="H86" s="11"/>
       <c r="I86" s="11"/>
     </row>
-    <row r="87" spans="2:9" ht="15.75" customHeight="1">
+    <row r="87" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B87" s="9"/>
       <c r="C87" s="10"/>
       <c r="D87" s="9"/>
@@ -2544,7 +2561,7 @@
       <c r="H87" s="11"/>
       <c r="I87" s="11"/>
     </row>
-    <row r="88" spans="2:9" ht="15.75" customHeight="1">
+    <row r="88" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B88" s="9"/>
       <c r="C88" s="10"/>
       <c r="D88" s="9"/>
@@ -2554,7 +2571,7 @@
       <c r="H88" s="11"/>
       <c r="I88" s="11"/>
     </row>
-    <row r="89" spans="2:9" ht="15.75" customHeight="1">
+    <row r="89" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B89" s="9"/>
       <c r="C89" s="10"/>
       <c r="D89" s="9"/>
@@ -2564,7 +2581,7 @@
       <c r="H89" s="11"/>
       <c r="I89" s="11"/>
     </row>
-    <row r="90" spans="2:9" ht="15.75" customHeight="1">
+    <row r="90" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B90" s="9"/>
       <c r="C90" s="10"/>
       <c r="D90" s="9"/>
@@ -2574,7 +2591,7 @@
       <c r="H90" s="11"/>
       <c r="I90" s="11"/>
     </row>
-    <row r="91" spans="2:9" ht="15.75" customHeight="1">
+    <row r="91" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B91" s="9"/>
       <c r="C91" s="10"/>
       <c r="D91" s="9"/>
@@ -2584,7 +2601,7 @@
       <c r="H91" s="11"/>
       <c r="I91" s="11"/>
     </row>
-    <row r="92" spans="2:9" ht="15.75" customHeight="1">
+    <row r="92" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B92" s="9"/>
       <c r="C92" s="10"/>
       <c r="D92" s="9"/>
@@ -2594,7 +2611,7 @@
       <c r="H92" s="11"/>
       <c r="I92" s="11"/>
     </row>
-    <row r="93" spans="2:9" ht="15.75" customHeight="1">
+    <row r="93" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B93" s="9"/>
       <c r="C93" s="10"/>
       <c r="D93" s="9"/>
@@ -2604,7 +2621,7 @@
       <c r="H93" s="11"/>
       <c r="I93" s="11"/>
     </row>
-    <row r="94" spans="2:9" ht="15.75" customHeight="1">
+    <row r="94" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B94" s="9"/>
       <c r="C94" s="10"/>
       <c r="D94" s="9"/>
@@ -2614,7 +2631,7 @@
       <c r="H94" s="11"/>
       <c r="I94" s="11"/>
     </row>
-    <row r="95" spans="2:9" ht="15.75" customHeight="1">
+    <row r="95" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B95" s="9"/>
       <c r="C95" s="10"/>
       <c r="D95" s="9"/>
@@ -2624,7 +2641,7 @@
       <c r="H95" s="11"/>
       <c r="I95" s="11"/>
     </row>
-    <row r="96" spans="2:9" ht="15.75" customHeight="1">
+    <row r="96" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B96" s="9"/>
       <c r="C96" s="10"/>
       <c r="D96" s="9"/>
@@ -2634,7 +2651,7 @@
       <c r="H96" s="11"/>
       <c r="I96" s="11"/>
     </row>
-    <row r="97" spans="2:9" ht="15.75" customHeight="1">
+    <row r="97" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B97" s="9"/>
       <c r="C97" s="10"/>
       <c r="D97" s="9"/>
@@ -2644,7 +2661,7 @@
       <c r="H97" s="11"/>
       <c r="I97" s="11"/>
     </row>
-    <row r="98" spans="2:9" ht="15.75" customHeight="1">
+    <row r="98" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B98" s="9"/>
       <c r="C98" s="10"/>
       <c r="D98" s="9"/>
@@ -2654,7 +2671,7 @@
       <c r="H98" s="11"/>
       <c r="I98" s="11"/>
     </row>
-    <row r="99" spans="2:9" ht="15.75" customHeight="1">
+    <row r="99" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B99" s="9"/>
       <c r="C99" s="10"/>
       <c r="D99" s="9"/>
@@ -2664,7 +2681,7 @@
       <c r="H99" s="11"/>
       <c r="I99" s="11"/>
     </row>
-    <row r="100" spans="2:9" ht="15.75" customHeight="1">
+    <row r="100" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B100" s="9"/>
       <c r="C100" s="10"/>
       <c r="D100" s="9"/>
@@ -2674,7 +2691,7 @@
       <c r="H100" s="11"/>
       <c r="I100" s="11"/>
     </row>
-    <row r="101" spans="2:9" ht="15.75" customHeight="1">
+    <row r="101" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B101" s="9"/>
       <c r="C101" s="10"/>
       <c r="D101" s="9"/>
@@ -2684,7 +2701,7 @@
       <c r="H101" s="11"/>
       <c r="I101" s="11"/>
     </row>
-    <row r="102" spans="2:9" ht="15.75" customHeight="1">
+    <row r="102" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B102" s="9"/>
       <c r="C102" s="10"/>
       <c r="D102" s="9"/>
@@ -2694,7 +2711,7 @@
       <c r="H102" s="11"/>
       <c r="I102" s="11"/>
     </row>
-    <row r="103" spans="2:9" ht="15.75" customHeight="1">
+    <row r="103" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B103" s="9"/>
       <c r="C103" s="10"/>
       <c r="D103" s="9"/>
@@ -2704,7 +2721,7 @@
       <c r="H103" s="11"/>
       <c r="I103" s="11"/>
     </row>
-    <row r="104" spans="2:9" ht="15.75" customHeight="1">
+    <row r="104" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B104" s="9"/>
       <c r="C104" s="10"/>
       <c r="D104" s="9"/>
@@ -2714,7 +2731,7 @@
       <c r="H104" s="11"/>
       <c r="I104" s="11"/>
     </row>
-    <row r="105" spans="2:9" ht="15.75" customHeight="1">
+    <row r="105" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B105" s="9"/>
       <c r="C105" s="10"/>
       <c r="D105" s="9"/>
@@ -2724,7 +2741,7 @@
       <c r="H105" s="11"/>
       <c r="I105" s="11"/>
     </row>
-    <row r="106" spans="2:9" ht="15.75" customHeight="1">
+    <row r="106" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B106" s="9"/>
       <c r="C106" s="10"/>
       <c r="D106" s="9"/>
@@ -2734,7 +2751,7 @@
       <c r="H106" s="11"/>
       <c r="I106" s="11"/>
     </row>
-    <row r="107" spans="2:9" ht="15.75" customHeight="1">
+    <row r="107" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B107" s="9"/>
       <c r="C107" s="10"/>
       <c r="D107" s="9"/>
@@ -2744,7 +2761,7 @@
       <c r="H107" s="11"/>
       <c r="I107" s="11"/>
     </row>
-    <row r="108" spans="2:9" ht="15.75" customHeight="1">
+    <row r="108" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B108" s="9"/>
       <c r="C108" s="10"/>
       <c r="D108" s="9"/>
@@ -2754,7 +2771,7 @@
       <c r="H108" s="11"/>
       <c r="I108" s="11"/>
     </row>
-    <row r="109" spans="2:9" ht="15.75" customHeight="1">
+    <row r="109" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B109" s="9"/>
       <c r="C109" s="10"/>
       <c r="D109" s="9"/>
@@ -2764,7 +2781,7 @@
       <c r="H109" s="11"/>
       <c r="I109" s="11"/>
     </row>
-    <row r="110" spans="2:9" ht="15.75" customHeight="1">
+    <row r="110" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B110" s="9"/>
       <c r="C110" s="10"/>
       <c r="D110" s="9"/>
@@ -2774,7 +2791,7 @@
       <c r="H110" s="11"/>
       <c r="I110" s="11"/>
     </row>
-    <row r="111" spans="2:9" ht="15.75" customHeight="1">
+    <row r="111" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B111" s="9"/>
       <c r="C111" s="10"/>
       <c r="D111" s="9"/>
@@ -2784,7 +2801,7 @@
       <c r="H111" s="11"/>
       <c r="I111" s="11"/>
     </row>
-    <row r="112" spans="2:9" ht="15.75" customHeight="1">
+    <row r="112" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B112" s="9"/>
       <c r="C112" s="10"/>
       <c r="D112" s="9"/>
@@ -2794,7 +2811,7 @@
       <c r="H112" s="11"/>
       <c r="I112" s="11"/>
     </row>
-    <row r="113" spans="2:9" ht="15.75" customHeight="1">
+    <row r="113" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B113" s="9"/>
       <c r="C113" s="10"/>
       <c r="D113" s="9"/>
@@ -2804,7 +2821,7 @@
       <c r="H113" s="11"/>
       <c r="I113" s="11"/>
     </row>
-    <row r="114" spans="2:9" ht="15.75" customHeight="1">
+    <row r="114" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B114" s="9"/>
       <c r="C114" s="10"/>
       <c r="D114" s="9"/>
@@ -2814,7 +2831,7 @@
       <c r="H114" s="11"/>
       <c r="I114" s="11"/>
     </row>
-    <row r="115" spans="2:9" ht="15.75" customHeight="1">
+    <row r="115" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B115" s="9"/>
       <c r="C115" s="10"/>
       <c r="D115" s="9"/>
@@ -2824,7 +2841,7 @@
       <c r="H115" s="11"/>
       <c r="I115" s="11"/>
     </row>
-    <row r="116" spans="2:9" ht="15.75" customHeight="1">
+    <row r="116" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B116" s="9"/>
       <c r="C116" s="10"/>
       <c r="D116" s="9"/>
@@ -2834,7 +2851,7 @@
       <c r="H116" s="11"/>
       <c r="I116" s="11"/>
     </row>
-    <row r="117" spans="2:9" ht="15.75" customHeight="1">
+    <row r="117" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B117" s="9"/>
       <c r="C117" s="10"/>
       <c r="D117" s="9"/>
@@ -2844,7 +2861,7 @@
       <c r="H117" s="11"/>
       <c r="I117" s="11"/>
     </row>
-    <row r="118" spans="2:9" ht="15.75" customHeight="1">
+    <row r="118" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B118" s="9"/>
       <c r="C118" s="10"/>
       <c r="D118" s="9"/>
@@ -2854,7 +2871,7 @@
       <c r="H118" s="11"/>
       <c r="I118" s="11"/>
     </row>
-    <row r="119" spans="2:9" ht="15.75" customHeight="1">
+    <row r="119" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B119" s="9"/>
       <c r="C119" s="10"/>
       <c r="D119" s="9"/>
@@ -2864,7 +2881,7 @@
       <c r="H119" s="11"/>
       <c r="I119" s="11"/>
     </row>
-    <row r="120" spans="2:9" ht="15.75" customHeight="1">
+    <row r="120" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B120" s="9"/>
       <c r="C120" s="10"/>
       <c r="D120" s="9"/>
@@ -2874,7 +2891,7 @@
       <c r="H120" s="11"/>
       <c r="I120" s="11"/>
     </row>
-    <row r="121" spans="2:9" ht="15.75" customHeight="1">
+    <row r="121" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B121" s="9"/>
       <c r="C121" s="10"/>
       <c r="D121" s="9"/>
@@ -2884,7 +2901,7 @@
       <c r="H121" s="11"/>
       <c r="I121" s="11"/>
     </row>
-    <row r="122" spans="2:9" ht="15.75" customHeight="1">
+    <row r="122" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B122" s="9"/>
       <c r="C122" s="10"/>
       <c r="D122" s="9"/>
@@ -2894,7 +2911,7 @@
       <c r="H122" s="11"/>
       <c r="I122" s="11"/>
     </row>
-    <row r="123" spans="2:9" ht="15.75" customHeight="1">
+    <row r="123" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B123" s="9"/>
       <c r="C123" s="10"/>
       <c r="D123" s="9"/>
@@ -2904,7 +2921,7 @@
       <c r="H123" s="11"/>
       <c r="I123" s="11"/>
     </row>
-    <row r="124" spans="2:9" ht="15.75" customHeight="1">
+    <row r="124" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B124" s="9"/>
       <c r="C124" s="10"/>
       <c r="D124" s="9"/>
@@ -2914,7 +2931,7 @@
       <c r="H124" s="11"/>
       <c r="I124" s="11"/>
     </row>
-    <row r="125" spans="2:9" ht="15.75" customHeight="1">
+    <row r="125" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B125" s="9"/>
       <c r="C125" s="10"/>
       <c r="D125" s="9"/>
@@ -2924,7 +2941,7 @@
       <c r="H125" s="11"/>
       <c r="I125" s="11"/>
     </row>
-    <row r="126" spans="2:9" ht="15.75" customHeight="1">
+    <row r="126" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B126" s="9"/>
       <c r="C126" s="10"/>
       <c r="D126" s="9"/>
@@ -2934,7 +2951,7 @@
       <c r="H126" s="11"/>
       <c r="I126" s="11"/>
     </row>
-    <row r="127" spans="2:9" ht="15.75" customHeight="1">
+    <row r="127" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B127" s="9"/>
       <c r="C127" s="10"/>
       <c r="D127" s="9"/>
@@ -2944,7 +2961,7 @@
       <c r="H127" s="11"/>
       <c r="I127" s="11"/>
     </row>
-    <row r="128" spans="2:9" ht="15.75" customHeight="1">
+    <row r="128" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B128" s="9"/>
       <c r="C128" s="10"/>
       <c r="D128" s="9"/>
@@ -2954,7 +2971,7 @@
       <c r="H128" s="11"/>
       <c r="I128" s="11"/>
     </row>
-    <row r="129" spans="2:9" ht="15.75" customHeight="1">
+    <row r="129" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B129" s="9"/>
       <c r="C129" s="10"/>
       <c r="D129" s="9"/>
@@ -2964,7 +2981,7 @@
       <c r="H129" s="11"/>
       <c r="I129" s="11"/>
     </row>
-    <row r="130" spans="2:9" ht="15.75" customHeight="1">
+    <row r="130" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B130" s="9"/>
       <c r="C130" s="10"/>
       <c r="D130" s="9"/>
@@ -2974,7 +2991,7 @@
       <c r="H130" s="11"/>
       <c r="I130" s="11"/>
     </row>
-    <row r="131" spans="2:9" ht="15.75" customHeight="1">
+    <row r="131" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B131" s="9"/>
       <c r="C131" s="10"/>
       <c r="D131" s="9"/>
@@ -2984,7 +3001,7 @@
       <c r="H131" s="11"/>
       <c r="I131" s="11"/>
     </row>
-    <row r="132" spans="2:9" ht="15.75" customHeight="1">
+    <row r="132" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B132" s="9"/>
       <c r="C132" s="10"/>
       <c r="D132" s="9"/>
@@ -2994,7 +3011,7 @@
       <c r="H132" s="11"/>
       <c r="I132" s="11"/>
     </row>
-    <row r="133" spans="2:9" ht="15.75" customHeight="1">
+    <row r="133" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B133" s="9"/>
       <c r="C133" s="10"/>
       <c r="D133" s="9"/>
@@ -3004,7 +3021,7 @@
       <c r="H133" s="11"/>
       <c r="I133" s="11"/>
     </row>
-    <row r="134" spans="2:9" ht="15.75" customHeight="1">
+    <row r="134" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B134" s="9"/>
       <c r="C134" s="10"/>
       <c r="D134" s="9"/>
@@ -3014,7 +3031,7 @@
       <c r="H134" s="11"/>
       <c r="I134" s="11"/>
     </row>
-    <row r="135" spans="2:9" ht="15.75" customHeight="1">
+    <row r="135" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B135" s="9"/>
       <c r="C135" s="10"/>
       <c r="D135" s="9"/>
@@ -3024,7 +3041,7 @@
       <c r="H135" s="11"/>
       <c r="I135" s="11"/>
     </row>
-    <row r="136" spans="2:9" ht="15.75" customHeight="1">
+    <row r="136" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B136" s="9"/>
       <c r="C136" s="10"/>
       <c r="D136" s="9"/>
@@ -3034,7 +3051,7 @@
       <c r="H136" s="11"/>
       <c r="I136" s="11"/>
     </row>
-    <row r="137" spans="2:9" ht="15.75" customHeight="1">
+    <row r="137" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B137" s="9"/>
       <c r="C137" s="10"/>
       <c r="D137" s="9"/>
@@ -3044,7 +3061,7 @@
       <c r="H137" s="11"/>
       <c r="I137" s="11"/>
     </row>
-    <row r="138" spans="2:9" ht="15.75" customHeight="1">
+    <row r="138" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B138" s="9"/>
       <c r="C138" s="10"/>
       <c r="D138" s="9"/>
@@ -3054,7 +3071,7 @@
       <c r="H138" s="11"/>
       <c r="I138" s="11"/>
     </row>
-    <row r="139" spans="2:9" ht="15.75" customHeight="1">
+    <row r="139" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B139" s="9"/>
       <c r="C139" s="10"/>
       <c r="D139" s="9"/>
@@ -3064,7 +3081,7 @@
       <c r="H139" s="11"/>
       <c r="I139" s="11"/>
     </row>
-    <row r="140" spans="2:9" ht="15.75" customHeight="1">
+    <row r="140" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B140" s="9"/>
       <c r="C140" s="10"/>
       <c r="D140" s="9"/>
@@ -3074,7 +3091,7 @@
       <c r="H140" s="11"/>
       <c r="I140" s="11"/>
     </row>
-    <row r="141" spans="2:9" ht="15.75" customHeight="1">
+    <row r="141" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B141" s="9"/>
       <c r="C141" s="10"/>
       <c r="D141" s="9"/>
@@ -3084,7 +3101,7 @@
       <c r="H141" s="11"/>
       <c r="I141" s="11"/>
     </row>
-    <row r="142" spans="2:9" ht="15.75" customHeight="1">
+    <row r="142" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B142" s="9"/>
       <c r="C142" s="10"/>
       <c r="D142" s="9"/>
@@ -3094,7 +3111,7 @@
       <c r="H142" s="11"/>
       <c r="I142" s="11"/>
     </row>
-    <row r="143" spans="2:9" ht="15.75" customHeight="1">
+    <row r="143" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B143" s="9"/>
       <c r="C143" s="10"/>
       <c r="D143" s="9"/>
@@ -3104,7 +3121,7 @@
       <c r="H143" s="11"/>
       <c r="I143" s="11"/>
     </row>
-    <row r="144" spans="2:9" ht="15.75" customHeight="1">
+    <row r="144" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B144" s="9"/>
       <c r="C144" s="10"/>
       <c r="D144" s="9"/>
@@ -3114,7 +3131,7 @@
       <c r="H144" s="11"/>
       <c r="I144" s="11"/>
     </row>
-    <row r="145" spans="2:9" ht="15.75" customHeight="1">
+    <row r="145" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B145" s="9"/>
       <c r="C145" s="10"/>
       <c r="D145" s="9"/>
@@ -3124,7 +3141,7 @@
       <c r="H145" s="11"/>
       <c r="I145" s="11"/>
     </row>
-    <row r="146" spans="2:9" ht="15.75" customHeight="1">
+    <row r="146" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B146" s="9"/>
       <c r="C146" s="10"/>
       <c r="D146" s="9"/>
@@ -3134,7 +3151,7 @@
       <c r="H146" s="11"/>
       <c r="I146" s="11"/>
     </row>
-    <row r="147" spans="2:9" ht="15.75" customHeight="1">
+    <row r="147" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B147" s="9"/>
       <c r="C147" s="10"/>
       <c r="D147" s="9"/>
@@ -3144,7 +3161,7 @@
       <c r="H147" s="11"/>
       <c r="I147" s="11"/>
     </row>
-    <row r="148" spans="2:9" ht="15.75" customHeight="1">
+    <row r="148" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B148" s="9"/>
       <c r="C148" s="10"/>
       <c r="D148" s="9"/>
@@ -3154,7 +3171,7 @@
       <c r="H148" s="11"/>
       <c r="I148" s="11"/>
     </row>
-    <row r="149" spans="2:9" ht="15.75" customHeight="1">
+    <row r="149" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B149" s="9"/>
       <c r="C149" s="10"/>
       <c r="D149" s="9"/>
@@ -3164,7 +3181,7 @@
       <c r="H149" s="11"/>
       <c r="I149" s="11"/>
     </row>
-    <row r="150" spans="2:9" ht="15.75" customHeight="1">
+    <row r="150" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B150" s="9"/>
       <c r="C150" s="10"/>
       <c r="D150" s="9"/>
@@ -3174,7 +3191,7 @@
       <c r="H150" s="11"/>
       <c r="I150" s="11"/>
     </row>
-    <row r="151" spans="2:9" ht="15.75" customHeight="1">
+    <row r="151" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B151" s="9"/>
       <c r="C151" s="10"/>
       <c r="D151" s="9"/>
@@ -3184,7 +3201,7 @@
       <c r="H151" s="11"/>
       <c r="I151" s="11"/>
     </row>
-    <row r="152" spans="2:9" ht="15.75" customHeight="1">
+    <row r="152" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B152" s="9"/>
       <c r="C152" s="10"/>
       <c r="D152" s="9"/>
@@ -3194,7 +3211,7 @@
       <c r="H152" s="11"/>
       <c r="I152" s="11"/>
     </row>
-    <row r="153" spans="2:9" ht="15.75" customHeight="1">
+    <row r="153" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B153" s="9"/>
       <c r="C153" s="10"/>
       <c r="D153" s="9"/>
@@ -3204,7 +3221,7 @@
       <c r="H153" s="11"/>
       <c r="I153" s="11"/>
     </row>
-    <row r="154" spans="2:9" ht="15.75" customHeight="1">
+    <row r="154" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B154" s="9"/>
       <c r="C154" s="10"/>
       <c r="D154" s="9"/>
@@ -3214,7 +3231,7 @@
       <c r="H154" s="11"/>
       <c r="I154" s="11"/>
     </row>
-    <row r="155" spans="2:9" ht="15.75" customHeight="1">
+    <row r="155" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B155" s="9"/>
       <c r="C155" s="10"/>
       <c r="D155" s="9"/>
@@ -3224,7 +3241,7 @@
       <c r="H155" s="11"/>
       <c r="I155" s="11"/>
     </row>
-    <row r="156" spans="2:9" ht="15.75" customHeight="1">
+    <row r="156" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B156" s="9"/>
       <c r="C156" s="10"/>
       <c r="D156" s="9"/>
@@ -3234,7 +3251,7 @@
       <c r="H156" s="11"/>
       <c r="I156" s="11"/>
     </row>
-    <row r="157" spans="2:9" ht="15.75" customHeight="1">
+    <row r="157" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B157" s="9"/>
       <c r="C157" s="10"/>
       <c r="D157" s="9"/>
@@ -3244,7 +3261,7 @@
       <c r="H157" s="11"/>
       <c r="I157" s="11"/>
     </row>
-    <row r="158" spans="2:9" ht="15.75" customHeight="1">
+    <row r="158" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B158" s="9"/>
       <c r="C158" s="10"/>
       <c r="D158" s="9"/>
@@ -3254,7 +3271,7 @@
       <c r="H158" s="11"/>
       <c r="I158" s="11"/>
     </row>
-    <row r="159" spans="2:9" ht="15.75" customHeight="1">
+    <row r="159" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B159" s="9"/>
       <c r="C159" s="10"/>
       <c r="D159" s="9"/>
@@ -3264,7 +3281,7 @@
       <c r="H159" s="11"/>
       <c r="I159" s="11"/>
     </row>
-    <row r="160" spans="2:9" ht="15.75" customHeight="1">
+    <row r="160" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B160" s="9"/>
       <c r="C160" s="10"/>
       <c r="D160" s="9"/>
@@ -3274,7 +3291,7 @@
       <c r="H160" s="11"/>
       <c r="I160" s="11"/>
     </row>
-    <row r="161" spans="2:9" ht="15.75" customHeight="1">
+    <row r="161" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B161" s="9"/>
       <c r="C161" s="10"/>
       <c r="D161" s="9"/>
@@ -3284,7 +3301,7 @@
       <c r="H161" s="11"/>
       <c r="I161" s="11"/>
     </row>
-    <row r="162" spans="2:9" ht="15.75" customHeight="1">
+    <row r="162" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B162" s="9"/>
       <c r="C162" s="10"/>
       <c r="D162" s="9"/>
@@ -3294,7 +3311,7 @@
       <c r="H162" s="11"/>
       <c r="I162" s="11"/>
     </row>
-    <row r="163" spans="2:9" ht="15.75" customHeight="1">
+    <row r="163" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B163" s="9"/>
       <c r="C163" s="10"/>
       <c r="D163" s="9"/>
@@ -3304,7 +3321,7 @@
       <c r="H163" s="11"/>
       <c r="I163" s="11"/>
     </row>
-    <row r="164" spans="2:9" ht="15.75" customHeight="1">
+    <row r="164" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B164" s="9"/>
       <c r="C164" s="10"/>
       <c r="D164" s="9"/>
@@ -3314,7 +3331,7 @@
       <c r="H164" s="11"/>
       <c r="I164" s="11"/>
     </row>
-    <row r="165" spans="2:9" ht="15.75" customHeight="1">
+    <row r="165" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B165" s="9"/>
       <c r="C165" s="10"/>
       <c r="D165" s="9"/>
@@ -3324,7 +3341,7 @@
       <c r="H165" s="11"/>
       <c r="I165" s="11"/>
     </row>
-    <row r="166" spans="2:9" ht="15.75" customHeight="1">
+    <row r="166" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B166" s="9"/>
       <c r="C166" s="10"/>
       <c r="D166" s="9"/>
@@ -3334,7 +3351,7 @@
       <c r="H166" s="11"/>
       <c r="I166" s="11"/>
     </row>
-    <row r="167" spans="2:9" ht="15.75" customHeight="1">
+    <row r="167" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B167" s="9"/>
       <c r="C167" s="10"/>
       <c r="D167" s="9"/>
@@ -3344,7 +3361,7 @@
       <c r="H167" s="11"/>
       <c r="I167" s="11"/>
     </row>
-    <row r="168" spans="2:9" ht="15.75" customHeight="1">
+    <row r="168" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B168" s="9"/>
       <c r="C168" s="10"/>
       <c r="D168" s="9"/>
@@ -3354,7 +3371,7 @@
       <c r="H168" s="11"/>
       <c r="I168" s="11"/>
     </row>
-    <row r="169" spans="2:9" ht="15.75" customHeight="1">
+    <row r="169" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B169" s="9"/>
       <c r="C169" s="10"/>
       <c r="D169" s="9"/>
@@ -3364,7 +3381,7 @@
       <c r="H169" s="11"/>
       <c r="I169" s="11"/>
     </row>
-    <row r="170" spans="2:9" ht="15.75" customHeight="1">
+    <row r="170" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B170" s="9"/>
       <c r="C170" s="10"/>
       <c r="D170" s="9"/>
@@ -3374,7 +3391,7 @@
       <c r="H170" s="11"/>
       <c r="I170" s="11"/>
     </row>
-    <row r="171" spans="2:9" ht="15.75" customHeight="1">
+    <row r="171" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B171" s="9"/>
       <c r="C171" s="10"/>
       <c r="D171" s="9"/>
@@ -3384,7 +3401,7 @@
       <c r="H171" s="11"/>
       <c r="I171" s="11"/>
     </row>
-    <row r="172" spans="2:9" ht="15.75" customHeight="1">
+    <row r="172" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B172" s="9"/>
       <c r="C172" s="10"/>
       <c r="D172" s="9"/>
@@ -3394,7 +3411,7 @@
       <c r="H172" s="11"/>
       <c r="I172" s="11"/>
     </row>
-    <row r="173" spans="2:9" ht="15.75" customHeight="1">
+    <row r="173" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B173" s="9"/>
       <c r="C173" s="10"/>
       <c r="D173" s="9"/>
@@ -3404,7 +3421,7 @@
       <c r="H173" s="11"/>
       <c r="I173" s="11"/>
     </row>
-    <row r="174" spans="2:9" ht="15.75" customHeight="1">
+    <row r="174" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B174" s="9"/>
       <c r="C174" s="10"/>
       <c r="D174" s="9"/>
@@ -3414,7 +3431,7 @@
       <c r="H174" s="11"/>
       <c r="I174" s="11"/>
     </row>
-    <row r="175" spans="2:9" ht="15.75" customHeight="1">
+    <row r="175" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B175" s="9"/>
       <c r="C175" s="10"/>
       <c r="D175" s="9"/>
@@ -3424,7 +3441,7 @@
       <c r="H175" s="11"/>
       <c r="I175" s="11"/>
     </row>
-    <row r="176" spans="2:9" ht="15.75" customHeight="1">
+    <row r="176" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B176" s="9"/>
       <c r="C176" s="10"/>
       <c r="D176" s="9"/>
@@ -3434,7 +3451,7 @@
       <c r="H176" s="11"/>
       <c r="I176" s="11"/>
     </row>
-    <row r="177" spans="2:9" ht="15.75" customHeight="1">
+    <row r="177" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B177" s="9"/>
       <c r="C177" s="10"/>
       <c r="D177" s="9"/>
@@ -3444,7 +3461,7 @@
       <c r="H177" s="11"/>
       <c r="I177" s="11"/>
     </row>
-    <row r="178" spans="2:9" ht="15.75" customHeight="1">
+    <row r="178" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B178" s="9"/>
       <c r="C178" s="10"/>
       <c r="D178" s="9"/>
@@ -3454,7 +3471,7 @@
       <c r="H178" s="11"/>
       <c r="I178" s="11"/>
     </row>
-    <row r="179" spans="2:9" ht="15.75" customHeight="1">
+    <row r="179" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B179" s="9"/>
       <c r="C179" s="10"/>
       <c r="D179" s="9"/>
@@ -3464,7 +3481,7 @@
       <c r="H179" s="11"/>
       <c r="I179" s="11"/>
     </row>
-    <row r="180" spans="2:9" ht="15.75" customHeight="1">
+    <row r="180" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B180" s="9"/>
       <c r="C180" s="10"/>
       <c r="D180" s="9"/>
@@ -3474,7 +3491,7 @@
       <c r="H180" s="11"/>
       <c r="I180" s="11"/>
     </row>
-    <row r="181" spans="2:9" ht="15.75" customHeight="1">
+    <row r="181" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B181" s="9"/>
       <c r="C181" s="10"/>
       <c r="D181" s="9"/>
@@ -3484,7 +3501,7 @@
       <c r="H181" s="11"/>
       <c r="I181" s="11"/>
     </row>
-    <row r="182" spans="2:9" ht="15.75" customHeight="1">
+    <row r="182" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B182" s="9"/>
       <c r="C182" s="10"/>
       <c r="D182" s="9"/>
@@ -3494,7 +3511,7 @@
       <c r="H182" s="11"/>
       <c r="I182" s="11"/>
     </row>
-    <row r="183" spans="2:9" ht="15.75" customHeight="1">
+    <row r="183" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B183" s="9"/>
       <c r="C183" s="10"/>
       <c r="D183" s="9"/>
@@ -3504,7 +3521,7 @@
       <c r="H183" s="11"/>
       <c r="I183" s="11"/>
     </row>
-    <row r="184" spans="2:9" ht="15.75" customHeight="1">
+    <row r="184" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B184" s="9"/>
       <c r="C184" s="10"/>
       <c r="D184" s="9"/>
@@ -3514,7 +3531,7 @@
       <c r="H184" s="11"/>
       <c r="I184" s="11"/>
     </row>
-    <row r="185" spans="2:9" ht="15.75" customHeight="1">
+    <row r="185" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B185" s="9"/>
       <c r="C185" s="10"/>
       <c r="D185" s="9"/>
@@ -3524,7 +3541,7 @@
       <c r="H185" s="11"/>
       <c r="I185" s="11"/>
     </row>
-    <row r="186" spans="2:9" ht="15.75" customHeight="1">
+    <row r="186" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B186" s="9"/>
       <c r="C186" s="10"/>
       <c r="D186" s="9"/>
@@ -3534,7 +3551,7 @@
       <c r="H186" s="11"/>
       <c r="I186" s="11"/>
     </row>
-    <row r="187" spans="2:9" ht="15.75" customHeight="1">
+    <row r="187" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B187" s="9"/>
       <c r="C187" s="10"/>
       <c r="D187" s="9"/>
@@ -3544,7 +3561,7 @@
       <c r="H187" s="11"/>
       <c r="I187" s="11"/>
     </row>
-    <row r="188" spans="2:9" ht="15.75" customHeight="1">
+    <row r="188" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B188" s="9"/>
       <c r="C188" s="10"/>
       <c r="D188" s="9"/>
@@ -3554,7 +3571,7 @@
       <c r="H188" s="11"/>
       <c r="I188" s="11"/>
     </row>
-    <row r="189" spans="2:9" ht="15.75" customHeight="1">
+    <row r="189" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B189" s="9"/>
       <c r="C189" s="10"/>
       <c r="D189" s="9"/>
@@ -3564,7 +3581,7 @@
       <c r="H189" s="11"/>
       <c r="I189" s="11"/>
     </row>
-    <row r="190" spans="2:9" ht="15.75" customHeight="1">
+    <row r="190" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B190" s="9"/>
       <c r="C190" s="10"/>
       <c r="D190" s="9"/>
@@ -3574,7 +3591,7 @@
       <c r="H190" s="11"/>
       <c r="I190" s="11"/>
     </row>
-    <row r="191" spans="2:9" ht="15.75" customHeight="1">
+    <row r="191" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B191" s="9"/>
       <c r="C191" s="10"/>
       <c r="D191" s="9"/>
@@ -3584,7 +3601,7 @@
       <c r="H191" s="11"/>
       <c r="I191" s="11"/>
     </row>
-    <row r="192" spans="2:9" ht="15.75" customHeight="1">
+    <row r="192" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B192" s="9"/>
       <c r="C192" s="10"/>
       <c r="D192" s="9"/>
@@ -3594,7 +3611,7 @@
       <c r="H192" s="11"/>
       <c r="I192" s="11"/>
     </row>
-    <row r="193" spans="2:9" ht="15.75" customHeight="1">
+    <row r="193" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B193" s="9"/>
       <c r="C193" s="10"/>
       <c r="D193" s="9"/>
@@ -3604,7 +3621,7 @@
       <c r="H193" s="11"/>
       <c r="I193" s="11"/>
     </row>
-    <row r="194" spans="2:9" ht="15.75" customHeight="1">
+    <row r="194" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B194" s="9"/>
       <c r="C194" s="10"/>
       <c r="D194" s="9"/>
@@ -3614,7 +3631,7 @@
       <c r="H194" s="11"/>
       <c r="I194" s="11"/>
     </row>
-    <row r="195" spans="2:9" ht="15.75" customHeight="1">
+    <row r="195" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B195" s="9"/>
       <c r="C195" s="10"/>
       <c r="D195" s="9"/>
@@ -3624,7 +3641,7 @@
       <c r="H195" s="11"/>
       <c r="I195" s="11"/>
     </row>
-    <row r="196" spans="2:9" ht="15.75" customHeight="1">
+    <row r="196" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B196" s="9"/>
       <c r="C196" s="10"/>
       <c r="D196" s="9"/>
@@ -3634,7 +3651,7 @@
       <c r="H196" s="11"/>
       <c r="I196" s="11"/>
     </row>
-    <row r="197" spans="2:9" ht="15.75" customHeight="1">
+    <row r="197" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B197" s="9"/>
       <c r="C197" s="10"/>
       <c r="D197" s="9"/>
@@ -3644,7 +3661,7 @@
       <c r="H197" s="11"/>
       <c r="I197" s="11"/>
     </row>
-    <row r="198" spans="2:9" ht="15.75" customHeight="1">
+    <row r="198" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B198" s="9"/>
       <c r="C198" s="10"/>
       <c r="D198" s="9"/>
@@ -3654,7 +3671,7 @@
       <c r="H198" s="11"/>
       <c r="I198" s="11"/>
     </row>
-    <row r="199" spans="2:9" ht="15.75" customHeight="1">
+    <row r="199" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B199" s="9"/>
       <c r="C199" s="10"/>
       <c r="D199" s="9"/>
@@ -3664,7 +3681,7 @@
       <c r="H199" s="11"/>
       <c r="I199" s="11"/>
     </row>
-    <row r="200" spans="2:9" ht="15.75" customHeight="1">
+    <row r="200" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B200" s="9"/>
       <c r="C200" s="10"/>
       <c r="D200" s="9"/>
@@ -3674,7 +3691,7 @@
       <c r="H200" s="11"/>
       <c r="I200" s="11"/>
     </row>
-    <row r="201" spans="2:9" ht="15.75" customHeight="1">
+    <row r="201" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B201" s="9"/>
       <c r="C201" s="10"/>
       <c r="D201" s="9"/>
@@ -3684,7 +3701,7 @@
       <c r="H201" s="11"/>
       <c r="I201" s="11"/>
     </row>
-    <row r="202" spans="2:9" ht="15.75" customHeight="1">
+    <row r="202" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B202" s="9"/>
       <c r="C202" s="10"/>
       <c r="D202" s="9"/>
@@ -3694,7 +3711,7 @@
       <c r="H202" s="11"/>
       <c r="I202" s="11"/>
     </row>
-    <row r="203" spans="2:9" ht="15.75" customHeight="1">
+    <row r="203" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B203" s="9"/>
       <c r="C203" s="10"/>
       <c r="D203" s="9"/>
@@ -3704,7 +3721,7 @@
       <c r="H203" s="11"/>
       <c r="I203" s="11"/>
     </row>
-    <row r="204" spans="2:9" ht="15.75" customHeight="1">
+    <row r="204" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B204" s="9"/>
       <c r="C204" s="10"/>
       <c r="D204" s="9"/>
@@ -3714,7 +3731,7 @@
       <c r="H204" s="11"/>
       <c r="I204" s="11"/>
     </row>
-    <row r="205" spans="2:9" ht="15.75" customHeight="1">
+    <row r="205" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B205" s="9"/>
       <c r="C205" s="10"/>
       <c r="D205" s="9"/>
@@ -3724,7 +3741,7 @@
       <c r="H205" s="11"/>
       <c r="I205" s="11"/>
     </row>
-    <row r="206" spans="2:9" ht="15.75" customHeight="1">
+    <row r="206" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B206" s="9"/>
       <c r="C206" s="10"/>
       <c r="D206" s="9"/>
@@ -3734,7 +3751,7 @@
       <c r="H206" s="11"/>
       <c r="I206" s="11"/>
     </row>
-    <row r="207" spans="2:9" ht="15.75" customHeight="1">
+    <row r="207" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B207" s="9"/>
       <c r="C207" s="10"/>
       <c r="D207" s="9"/>
@@ -3744,7 +3761,7 @@
       <c r="H207" s="11"/>
       <c r="I207" s="11"/>
     </row>
-    <row r="208" spans="2:9" ht="15.75" customHeight="1">
+    <row r="208" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B208" s="9"/>
       <c r="C208" s="10"/>
       <c r="D208" s="9"/>
@@ -3754,7 +3771,7 @@
       <c r="H208" s="11"/>
       <c r="I208" s="11"/>
     </row>
-    <row r="209" spans="2:9" ht="15.75" customHeight="1">
+    <row r="209" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B209" s="9"/>
       <c r="C209" s="10"/>
       <c r="D209" s="9"/>
@@ -3764,7 +3781,7 @@
       <c r="H209" s="11"/>
       <c r="I209" s="11"/>
     </row>
-    <row r="210" spans="2:9" ht="15.75" customHeight="1">
+    <row r="210" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B210" s="9"/>
       <c r="C210" s="10"/>
       <c r="D210" s="9"/>
@@ -3774,7 +3791,7 @@
       <c r="H210" s="11"/>
       <c r="I210" s="11"/>
     </row>
-    <row r="211" spans="2:9" ht="15.75" customHeight="1">
+    <row r="211" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B211" s="9"/>
       <c r="C211" s="10"/>
       <c r="D211" s="9"/>
@@ -3784,7 +3801,7 @@
       <c r="H211" s="11"/>
       <c r="I211" s="11"/>
     </row>
-    <row r="212" spans="2:9" ht="15.75" customHeight="1">
+    <row r="212" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B212" s="9"/>
       <c r="C212" s="10"/>
       <c r="D212" s="9"/>
@@ -3794,7 +3811,7 @@
       <c r="H212" s="11"/>
       <c r="I212" s="11"/>
     </row>
-    <row r="213" spans="2:9" ht="15.75" customHeight="1">
+    <row r="213" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B213" s="9"/>
       <c r="C213" s="10"/>
       <c r="D213" s="9"/>
@@ -3804,7 +3821,7 @@
       <c r="H213" s="11"/>
       <c r="I213" s="11"/>
     </row>
-    <row r="214" spans="2:9" ht="15.75" customHeight="1">
+    <row r="214" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B214" s="9"/>
       <c r="C214" s="10"/>
       <c r="D214" s="9"/>
@@ -3814,7 +3831,7 @@
       <c r="H214" s="11"/>
       <c r="I214" s="11"/>
     </row>
-    <row r="215" spans="2:9" ht="15.75" customHeight="1">
+    <row r="215" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B215" s="9"/>
       <c r="C215" s="10"/>
       <c r="D215" s="9"/>
@@ -3824,7 +3841,7 @@
       <c r="H215" s="11"/>
       <c r="I215" s="11"/>
     </row>
-    <row r="216" spans="2:9" ht="15.75" customHeight="1">
+    <row r="216" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B216" s="9"/>
       <c r="C216" s="10"/>
       <c r="D216" s="9"/>
@@ -3834,7 +3851,7 @@
       <c r="H216" s="11"/>
       <c r="I216" s="11"/>
     </row>
-    <row r="217" spans="2:9" ht="15.75" customHeight="1">
+    <row r="217" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B217" s="9"/>
       <c r="C217" s="10"/>
       <c r="D217" s="9"/>
@@ -3844,7 +3861,7 @@
       <c r="H217" s="11"/>
       <c r="I217" s="11"/>
     </row>
-    <row r="218" spans="2:9" ht="15.75" customHeight="1">
+    <row r="218" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B218" s="9"/>
       <c r="C218" s="10"/>
       <c r="D218" s="9"/>
@@ -3854,7 +3871,7 @@
       <c r="H218" s="11"/>
       <c r="I218" s="11"/>
     </row>
-    <row r="219" spans="2:9" ht="15.75" customHeight="1">
+    <row r="219" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B219" s="9"/>
       <c r="C219" s="10"/>
       <c r="D219" s="9"/>
@@ -3864,7 +3881,7 @@
       <c r="H219" s="11"/>
       <c r="I219" s="11"/>
     </row>
-    <row r="220" spans="2:9" ht="15.75" customHeight="1">
+    <row r="220" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B220" s="9"/>
       <c r="C220" s="10"/>
       <c r="D220" s="9"/>
@@ -3874,7 +3891,7 @@
       <c r="H220" s="11"/>
       <c r="I220" s="11"/>
     </row>
-    <row r="221" spans="2:9" ht="15.75" customHeight="1">
+    <row r="221" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B221" s="9"/>
       <c r="C221" s="10"/>
       <c r="D221" s="9"/>
@@ -3884,7 +3901,7 @@
       <c r="H221" s="11"/>
       <c r="I221" s="11"/>
     </row>
-    <row r="222" spans="2:9" ht="15.75" customHeight="1">
+    <row r="222" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B222" s="9"/>
       <c r="C222" s="10"/>
       <c r="D222" s="9"/>
@@ -3894,7 +3911,7 @@
       <c r="H222" s="11"/>
       <c r="I222" s="11"/>
     </row>
-    <row r="223" spans="2:9" ht="15.75" customHeight="1">
+    <row r="223" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B223" s="9"/>
       <c r="C223" s="10"/>
       <c r="D223" s="9"/>
@@ -3904,7 +3921,7 @@
       <c r="H223" s="11"/>
       <c r="I223" s="11"/>
     </row>
-    <row r="224" spans="2:9" ht="15.75" customHeight="1">
+    <row r="224" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B224" s="9"/>
       <c r="C224" s="10"/>
       <c r="D224" s="9"/>
@@ -3914,7 +3931,7 @@
       <c r="H224" s="11"/>
       <c r="I224" s="11"/>
     </row>
-    <row r="225" spans="2:9" ht="15.75" customHeight="1">
+    <row r="225" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B225" s="9"/>
       <c r="C225" s="10"/>
       <c r="D225" s="9"/>
@@ -3924,7 +3941,7 @@
       <c r="H225" s="11"/>
       <c r="I225" s="11"/>
     </row>
-    <row r="226" spans="2:9" ht="15.75" customHeight="1">
+    <row r="226" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B226" s="9"/>
       <c r="C226" s="10"/>
       <c r="D226" s="9"/>
@@ -3934,7 +3951,7 @@
       <c r="H226" s="11"/>
       <c r="I226" s="11"/>
     </row>
-    <row r="227" spans="2:9" ht="15.75" customHeight="1">
+    <row r="227" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B227" s="9"/>
       <c r="C227" s="10"/>
       <c r="D227" s="9"/>
@@ -3944,7 +3961,7 @@
       <c r="H227" s="11"/>
       <c r="I227" s="11"/>
     </row>
-    <row r="228" spans="2:9" ht="15.75" customHeight="1">
+    <row r="228" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B228" s="9"/>
       <c r="C228" s="10"/>
       <c r="D228" s="9"/>
@@ -3954,778 +3971,778 @@
       <c r="H228" s="11"/>
       <c r="I228" s="11"/>
     </row>
-    <row r="229" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="230" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="231" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="232" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="233" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="234" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="235" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="236" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="237" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="238" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="239" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="240" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="241" ht="15.75" customHeight="1"/>
-    <row r="242" ht="15.75" customHeight="1"/>
-    <row r="243" ht="15.75" customHeight="1"/>
-    <row r="244" ht="15.75" customHeight="1"/>
-    <row r="245" ht="15.75" customHeight="1"/>
-    <row r="246" ht="15.75" customHeight="1"/>
-    <row r="247" ht="15.75" customHeight="1"/>
-    <row r="248" ht="15.75" customHeight="1"/>
-    <row r="249" ht="15.75" customHeight="1"/>
-    <row r="250" ht="15.75" customHeight="1"/>
-    <row r="251" ht="15.75" customHeight="1"/>
-    <row r="252" ht="15.75" customHeight="1"/>
-    <row r="253" ht="15.75" customHeight="1"/>
-    <row r="254" ht="15.75" customHeight="1"/>
-    <row r="255" ht="15.75" customHeight="1"/>
-    <row r="256" ht="15.75" customHeight="1"/>
-    <row r="257" ht="15.75" customHeight="1"/>
-    <row r="258" ht="15.75" customHeight="1"/>
-    <row r="259" ht="15.75" customHeight="1"/>
-    <row r="260" ht="15.75" customHeight="1"/>
-    <row r="261" ht="15.75" customHeight="1"/>
-    <row r="262" ht="15.75" customHeight="1"/>
-    <row r="263" ht="15.75" customHeight="1"/>
-    <row r="264" ht="15.75" customHeight="1"/>
-    <row r="265" ht="15.75" customHeight="1"/>
-    <row r="266" ht="15.75" customHeight="1"/>
-    <row r="267" ht="15.75" customHeight="1"/>
-    <row r="268" ht="15.75" customHeight="1"/>
-    <row r="269" ht="15.75" customHeight="1"/>
-    <row r="270" ht="15.75" customHeight="1"/>
-    <row r="271" ht="15.75" customHeight="1"/>
-    <row r="272" ht="15.75" customHeight="1"/>
-    <row r="273" ht="15.75" customHeight="1"/>
-    <row r="274" ht="15.75" customHeight="1"/>
-    <row r="275" ht="15.75" customHeight="1"/>
-    <row r="276" ht="15.75" customHeight="1"/>
-    <row r="277" ht="15.75" customHeight="1"/>
-    <row r="278" ht="15.75" customHeight="1"/>
-    <row r="279" ht="15.75" customHeight="1"/>
-    <row r="280" ht="15.75" customHeight="1"/>
-    <row r="281" ht="15.75" customHeight="1"/>
-    <row r="282" ht="15.75" customHeight="1"/>
-    <row r="283" ht="15.75" customHeight="1"/>
-    <row r="284" ht="15.75" customHeight="1"/>
-    <row r="285" ht="15.75" customHeight="1"/>
-    <row r="286" ht="15.75" customHeight="1"/>
-    <row r="287" ht="15.75" customHeight="1"/>
-    <row r="288" ht="15.75" customHeight="1"/>
-    <row r="289" ht="15.75" customHeight="1"/>
-    <row r="290" ht="15.75" customHeight="1"/>
-    <row r="291" ht="15.75" customHeight="1"/>
-    <row r="292" ht="15.75" customHeight="1"/>
-    <row r="293" ht="15.75" customHeight="1"/>
-    <row r="294" ht="15.75" customHeight="1"/>
-    <row r="295" ht="15.75" customHeight="1"/>
-    <row r="296" ht="15.75" customHeight="1"/>
-    <row r="297" ht="15.75" customHeight="1"/>
-    <row r="298" ht="15.75" customHeight="1"/>
-    <row r="299" ht="15.75" customHeight="1"/>
-    <row r="300" ht="15.75" customHeight="1"/>
-    <row r="301" ht="15.75" customHeight="1"/>
-    <row r="302" ht="15.75" customHeight="1"/>
-    <row r="303" ht="15.75" customHeight="1"/>
-    <row r="304" ht="15.75" customHeight="1"/>
-    <row r="305" ht="15.75" customHeight="1"/>
-    <row r="306" ht="15.75" customHeight="1"/>
-    <row r="307" ht="15.75" customHeight="1"/>
-    <row r="308" ht="15.75" customHeight="1"/>
-    <row r="309" ht="15.75" customHeight="1"/>
-    <row r="310" ht="15.75" customHeight="1"/>
-    <row r="311" ht="15.75" customHeight="1"/>
-    <row r="312" ht="15.75" customHeight="1"/>
-    <row r="313" ht="15.75" customHeight="1"/>
-    <row r="314" ht="15.75" customHeight="1"/>
-    <row r="315" ht="15.75" customHeight="1"/>
-    <row r="316" ht="15.75" customHeight="1"/>
-    <row r="317" ht="15.75" customHeight="1"/>
-    <row r="318" ht="15.75" customHeight="1"/>
-    <row r="319" ht="15.75" customHeight="1"/>
-    <row r="320" ht="15.75" customHeight="1"/>
-    <row r="321" ht="15.75" customHeight="1"/>
-    <row r="322" ht="15.75" customHeight="1"/>
-    <row r="323" ht="15.75" customHeight="1"/>
-    <row r="324" ht="15.75" customHeight="1"/>
-    <row r="325" ht="15.75" customHeight="1"/>
-    <row r="326" ht="15.75" customHeight="1"/>
-    <row r="327" ht="15.75" customHeight="1"/>
-    <row r="328" ht="15.75" customHeight="1"/>
-    <row r="329" ht="15.75" customHeight="1"/>
-    <row r="330" ht="15.75" customHeight="1"/>
-    <row r="331" ht="15.75" customHeight="1"/>
-    <row r="332" ht="15.75" customHeight="1"/>
-    <row r="333" ht="15.75" customHeight="1"/>
-    <row r="334" ht="15.75" customHeight="1"/>
-    <row r="335" ht="15.75" customHeight="1"/>
-    <row r="336" ht="15.75" customHeight="1"/>
-    <row r="337" ht="15.75" customHeight="1"/>
-    <row r="338" ht="15.75" customHeight="1"/>
-    <row r="339" ht="15.75" customHeight="1"/>
-    <row r="340" ht="15.75" customHeight="1"/>
-    <row r="341" ht="15.75" customHeight="1"/>
-    <row r="342" ht="15.75" customHeight="1"/>
-    <row r="343" ht="15.75" customHeight="1"/>
-    <row r="344" ht="15.75" customHeight="1"/>
-    <row r="345" ht="15.75" customHeight="1"/>
-    <row r="346" ht="15.75" customHeight="1"/>
-    <row r="347" ht="15.75" customHeight="1"/>
-    <row r="348" ht="15.75" customHeight="1"/>
-    <row r="349" ht="15.75" customHeight="1"/>
-    <row r="350" ht="15.75" customHeight="1"/>
-    <row r="351" ht="15.75" customHeight="1"/>
-    <row r="352" ht="15.75" customHeight="1"/>
-    <row r="353" ht="15.75" customHeight="1"/>
-    <row r="354" ht="15.75" customHeight="1"/>
-    <row r="355" ht="15.75" customHeight="1"/>
-    <row r="356" ht="15.75" customHeight="1"/>
-    <row r="357" ht="15.75" customHeight="1"/>
-    <row r="358" ht="15.75" customHeight="1"/>
-    <row r="359" ht="15.75" customHeight="1"/>
-    <row r="360" ht="15.75" customHeight="1"/>
-    <row r="361" ht="15.75" customHeight="1"/>
-    <row r="362" ht="15.75" customHeight="1"/>
-    <row r="363" ht="15.75" customHeight="1"/>
-    <row r="364" ht="15.75" customHeight="1"/>
-    <row r="365" ht="15.75" customHeight="1"/>
-    <row r="366" ht="15.75" customHeight="1"/>
-    <row r="367" ht="15.75" customHeight="1"/>
-    <row r="368" ht="15.75" customHeight="1"/>
-    <row r="369" ht="15.75" customHeight="1"/>
-    <row r="370" ht="15.75" customHeight="1"/>
-    <row r="371" ht="15.75" customHeight="1"/>
-    <row r="372" ht="15.75" customHeight="1"/>
-    <row r="373" ht="15.75" customHeight="1"/>
-    <row r="374" ht="15.75" customHeight="1"/>
-    <row r="375" ht="15.75" customHeight="1"/>
-    <row r="376" ht="15.75" customHeight="1"/>
-    <row r="377" ht="15.75" customHeight="1"/>
-    <row r="378" ht="15.75" customHeight="1"/>
-    <row r="379" ht="15.75" customHeight="1"/>
-    <row r="380" ht="15.75" customHeight="1"/>
-    <row r="381" ht="15.75" customHeight="1"/>
-    <row r="382" ht="15.75" customHeight="1"/>
-    <row r="383" ht="15.75" customHeight="1"/>
-    <row r="384" ht="15.75" customHeight="1"/>
-    <row r="385" ht="15.75" customHeight="1"/>
-    <row r="386" ht="15.75" customHeight="1"/>
-    <row r="387" ht="15.75" customHeight="1"/>
-    <row r="388" ht="15.75" customHeight="1"/>
-    <row r="389" ht="15.75" customHeight="1"/>
-    <row r="390" ht="15.75" customHeight="1"/>
-    <row r="391" ht="15.75" customHeight="1"/>
-    <row r="392" ht="15.75" customHeight="1"/>
-    <row r="393" ht="15.75" customHeight="1"/>
-    <row r="394" ht="15.75" customHeight="1"/>
-    <row r="395" ht="15.75" customHeight="1"/>
-    <row r="396" ht="15.75" customHeight="1"/>
-    <row r="397" ht="15.75" customHeight="1"/>
-    <row r="398" ht="15.75" customHeight="1"/>
-    <row r="399" ht="15.75" customHeight="1"/>
-    <row r="400" ht="15.75" customHeight="1"/>
-    <row r="401" ht="15.75" customHeight="1"/>
-    <row r="402" ht="15.75" customHeight="1"/>
-    <row r="403" ht="15.75" customHeight="1"/>
-    <row r="404" ht="15.75" customHeight="1"/>
-    <row r="405" ht="15.75" customHeight="1"/>
-    <row r="406" ht="15.75" customHeight="1"/>
-    <row r="407" ht="15.75" customHeight="1"/>
-    <row r="408" ht="15.75" customHeight="1"/>
-    <row r="409" ht="15.75" customHeight="1"/>
-    <row r="410" ht="15.75" customHeight="1"/>
-    <row r="411" ht="15.75" customHeight="1"/>
-    <row r="412" ht="15.75" customHeight="1"/>
-    <row r="413" ht="15.75" customHeight="1"/>
-    <row r="414" ht="15.75" customHeight="1"/>
-    <row r="415" ht="15.75" customHeight="1"/>
-    <row r="416" ht="15.75" customHeight="1"/>
-    <row r="417" ht="15.75" customHeight="1"/>
-    <row r="418" ht="15.75" customHeight="1"/>
-    <row r="419" ht="15.75" customHeight="1"/>
-    <row r="420" ht="15.75" customHeight="1"/>
-    <row r="421" ht="15.75" customHeight="1"/>
-    <row r="422" ht="15.75" customHeight="1"/>
-    <row r="423" ht="15.75" customHeight="1"/>
-    <row r="424" ht="15.75" customHeight="1"/>
-    <row r="425" ht="15.75" customHeight="1"/>
-    <row r="426" ht="15.75" customHeight="1"/>
-    <row r="427" ht="15.75" customHeight="1"/>
-    <row r="428" ht="15.75" customHeight="1"/>
-    <row r="429" ht="15.75" customHeight="1"/>
-    <row r="430" ht="15.75" customHeight="1"/>
-    <row r="431" ht="15.75" customHeight="1"/>
-    <row r="432" ht="15.75" customHeight="1"/>
-    <row r="433" ht="15.75" customHeight="1"/>
-    <row r="434" ht="15.75" customHeight="1"/>
-    <row r="435" ht="15.75" customHeight="1"/>
-    <row r="436" ht="15.75" customHeight="1"/>
-    <row r="437" ht="15.75" customHeight="1"/>
-    <row r="438" ht="15.75" customHeight="1"/>
-    <row r="439" ht="15.75" customHeight="1"/>
-    <row r="440" ht="15.75" customHeight="1"/>
-    <row r="441" ht="15.75" customHeight="1"/>
-    <row r="442" ht="15.75" customHeight="1"/>
-    <row r="443" ht="15.75" customHeight="1"/>
-    <row r="444" ht="15.75" customHeight="1"/>
-    <row r="445" ht="15.75" customHeight="1"/>
-    <row r="446" ht="15.75" customHeight="1"/>
-    <row r="447" ht="15.75" customHeight="1"/>
-    <row r="448" ht="15.75" customHeight="1"/>
-    <row r="449" ht="15.75" customHeight="1"/>
-    <row r="450" ht="15.75" customHeight="1"/>
-    <row r="451" ht="15.75" customHeight="1"/>
-    <row r="452" ht="15.75" customHeight="1"/>
-    <row r="453" ht="15.75" customHeight="1"/>
-    <row r="454" ht="15.75" customHeight="1"/>
-    <row r="455" ht="15.75" customHeight="1"/>
-    <row r="456" ht="15.75" customHeight="1"/>
-    <row r="457" ht="15.75" customHeight="1"/>
-    <row r="458" ht="15.75" customHeight="1"/>
-    <row r="459" ht="15.75" customHeight="1"/>
-    <row r="460" ht="15.75" customHeight="1"/>
-    <row r="461" ht="15.75" customHeight="1"/>
-    <row r="462" ht="15.75" customHeight="1"/>
-    <row r="463" ht="15.75" customHeight="1"/>
-    <row r="464" ht="15.75" customHeight="1"/>
-    <row r="465" ht="15.75" customHeight="1"/>
-    <row r="466" ht="15.75" customHeight="1"/>
-    <row r="467" ht="15.75" customHeight="1"/>
-    <row r="468" ht="15.75" customHeight="1"/>
-    <row r="469" ht="15.75" customHeight="1"/>
-    <row r="470" ht="15.75" customHeight="1"/>
-    <row r="471" ht="15.75" customHeight="1"/>
-    <row r="472" ht="15.75" customHeight="1"/>
-    <row r="473" ht="15.75" customHeight="1"/>
-    <row r="474" ht="15.75" customHeight="1"/>
-    <row r="475" ht="15.75" customHeight="1"/>
-    <row r="476" ht="15.75" customHeight="1"/>
-    <row r="477" ht="15.75" customHeight="1"/>
-    <row r="478" ht="15.75" customHeight="1"/>
-    <row r="479" ht="15.75" customHeight="1"/>
-    <row r="480" ht="15.75" customHeight="1"/>
-    <row r="481" ht="15.75" customHeight="1"/>
-    <row r="482" ht="15.75" customHeight="1"/>
-    <row r="483" ht="15.75" customHeight="1"/>
-    <row r="484" ht="15.75" customHeight="1"/>
-    <row r="485" ht="15.75" customHeight="1"/>
-    <row r="486" ht="15.75" customHeight="1"/>
-    <row r="487" ht="15.75" customHeight="1"/>
-    <row r="488" ht="15.75" customHeight="1"/>
-    <row r="489" ht="15.75" customHeight="1"/>
-    <row r="490" ht="15.75" customHeight="1"/>
-    <row r="491" ht="15.75" customHeight="1"/>
-    <row r="492" ht="15.75" customHeight="1"/>
-    <row r="493" ht="15.75" customHeight="1"/>
-    <row r="494" ht="15.75" customHeight="1"/>
-    <row r="495" ht="15.75" customHeight="1"/>
-    <row r="496" ht="15.75" customHeight="1"/>
-    <row r="497" ht="15.75" customHeight="1"/>
-    <row r="498" ht="15.75" customHeight="1"/>
-    <row r="499" ht="15.75" customHeight="1"/>
-    <row r="500" ht="15.75" customHeight="1"/>
-    <row r="501" ht="15.75" customHeight="1"/>
-    <row r="502" ht="15.75" customHeight="1"/>
-    <row r="503" ht="15.75" customHeight="1"/>
-    <row r="504" ht="15.75" customHeight="1"/>
-    <row r="505" ht="15.75" customHeight="1"/>
-    <row r="506" ht="15.75" customHeight="1"/>
-    <row r="507" ht="15.75" customHeight="1"/>
-    <row r="508" ht="15.75" customHeight="1"/>
-    <row r="509" ht="15.75" customHeight="1"/>
-    <row r="510" ht="15.75" customHeight="1"/>
-    <row r="511" ht="15.75" customHeight="1"/>
-    <row r="512" ht="15.75" customHeight="1"/>
-    <row r="513" ht="15.75" customHeight="1"/>
-    <row r="514" ht="15.75" customHeight="1"/>
-    <row r="515" ht="15.75" customHeight="1"/>
-    <row r="516" ht="15.75" customHeight="1"/>
-    <row r="517" ht="15.75" customHeight="1"/>
-    <row r="518" ht="15.75" customHeight="1"/>
-    <row r="519" ht="15.75" customHeight="1"/>
-    <row r="520" ht="15.75" customHeight="1"/>
-    <row r="521" ht="15.75" customHeight="1"/>
-    <row r="522" ht="15.75" customHeight="1"/>
-    <row r="523" ht="15.75" customHeight="1"/>
-    <row r="524" ht="15.75" customHeight="1"/>
-    <row r="525" ht="15.75" customHeight="1"/>
-    <row r="526" ht="15.75" customHeight="1"/>
-    <row r="527" ht="15.75" customHeight="1"/>
-    <row r="528" ht="15.75" customHeight="1"/>
-    <row r="529" ht="15.75" customHeight="1"/>
-    <row r="530" ht="15.75" customHeight="1"/>
-    <row r="531" ht="15.75" customHeight="1"/>
-    <row r="532" ht="15.75" customHeight="1"/>
-    <row r="533" ht="15.75" customHeight="1"/>
-    <row r="534" ht="15.75" customHeight="1"/>
-    <row r="535" ht="15.75" customHeight="1"/>
-    <row r="536" ht="15.75" customHeight="1"/>
-    <row r="537" ht="15.75" customHeight="1"/>
-    <row r="538" ht="15.75" customHeight="1"/>
-    <row r="539" ht="15.75" customHeight="1"/>
-    <row r="540" ht="15.75" customHeight="1"/>
-    <row r="541" ht="15.75" customHeight="1"/>
-    <row r="542" ht="15.75" customHeight="1"/>
-    <row r="543" ht="15.75" customHeight="1"/>
-    <row r="544" ht="15.75" customHeight="1"/>
-    <row r="545" ht="15.75" customHeight="1"/>
-    <row r="546" ht="15.75" customHeight="1"/>
-    <row r="547" ht="15.75" customHeight="1"/>
-    <row r="548" ht="15.75" customHeight="1"/>
-    <row r="549" ht="15.75" customHeight="1"/>
-    <row r="550" ht="15.75" customHeight="1"/>
-    <row r="551" ht="15.75" customHeight="1"/>
-    <row r="552" ht="15.75" customHeight="1"/>
-    <row r="553" ht="15.75" customHeight="1"/>
-    <row r="554" ht="15.75" customHeight="1"/>
-    <row r="555" ht="15.75" customHeight="1"/>
-    <row r="556" ht="15.75" customHeight="1"/>
-    <row r="557" ht="15.75" customHeight="1"/>
-    <row r="558" ht="15.75" customHeight="1"/>
-    <row r="559" ht="15.75" customHeight="1"/>
-    <row r="560" ht="15.75" customHeight="1"/>
-    <row r="561" ht="15.75" customHeight="1"/>
-    <row r="562" ht="15.75" customHeight="1"/>
-    <row r="563" ht="15.75" customHeight="1"/>
-    <row r="564" ht="15.75" customHeight="1"/>
-    <row r="565" ht="15.75" customHeight="1"/>
-    <row r="566" ht="15.75" customHeight="1"/>
-    <row r="567" ht="15.75" customHeight="1"/>
-    <row r="568" ht="15.75" customHeight="1"/>
-    <row r="569" ht="15.75" customHeight="1"/>
-    <row r="570" ht="15.75" customHeight="1"/>
-    <row r="571" ht="15.75" customHeight="1"/>
-    <row r="572" ht="15.75" customHeight="1"/>
-    <row r="573" ht="15.75" customHeight="1"/>
-    <row r="574" ht="15.75" customHeight="1"/>
-    <row r="575" ht="15.75" customHeight="1"/>
-    <row r="576" ht="15.75" customHeight="1"/>
-    <row r="577" ht="15.75" customHeight="1"/>
-    <row r="578" ht="15.75" customHeight="1"/>
-    <row r="579" ht="15.75" customHeight="1"/>
-    <row r="580" ht="15.75" customHeight="1"/>
-    <row r="581" ht="15.75" customHeight="1"/>
-    <row r="582" ht="15.75" customHeight="1"/>
-    <row r="583" ht="15.75" customHeight="1"/>
-    <row r="584" ht="15.75" customHeight="1"/>
-    <row r="585" ht="15.75" customHeight="1"/>
-    <row r="586" ht="15.75" customHeight="1"/>
-    <row r="587" ht="15.75" customHeight="1"/>
-    <row r="588" ht="15.75" customHeight="1"/>
-    <row r="589" ht="15.75" customHeight="1"/>
-    <row r="590" ht="15.75" customHeight="1"/>
-    <row r="591" ht="15.75" customHeight="1"/>
-    <row r="592" ht="15.75" customHeight="1"/>
-    <row r="593" ht="15.75" customHeight="1"/>
-    <row r="594" ht="15.75" customHeight="1"/>
-    <row r="595" ht="15.75" customHeight="1"/>
-    <row r="596" ht="15.75" customHeight="1"/>
-    <row r="597" ht="15.75" customHeight="1"/>
-    <row r="598" ht="15.75" customHeight="1"/>
-    <row r="599" ht="15.75" customHeight="1"/>
-    <row r="600" ht="15.75" customHeight="1"/>
-    <row r="601" ht="15.75" customHeight="1"/>
-    <row r="602" ht="15.75" customHeight="1"/>
-    <row r="603" ht="15.75" customHeight="1"/>
-    <row r="604" ht="15.75" customHeight="1"/>
-    <row r="605" ht="15.75" customHeight="1"/>
-    <row r="606" ht="15.75" customHeight="1"/>
-    <row r="607" ht="15.75" customHeight="1"/>
-    <row r="608" ht="15.75" customHeight="1"/>
-    <row r="609" ht="15.75" customHeight="1"/>
-    <row r="610" ht="15.75" customHeight="1"/>
-    <row r="611" ht="15.75" customHeight="1"/>
-    <row r="612" ht="15.75" customHeight="1"/>
-    <row r="613" ht="15.75" customHeight="1"/>
-    <row r="614" ht="15.75" customHeight="1"/>
-    <row r="615" ht="15.75" customHeight="1"/>
-    <row r="616" ht="15.75" customHeight="1"/>
-    <row r="617" ht="15.75" customHeight="1"/>
-    <row r="618" ht="15.75" customHeight="1"/>
-    <row r="619" ht="15.75" customHeight="1"/>
-    <row r="620" ht="15.75" customHeight="1"/>
-    <row r="621" ht="15.75" customHeight="1"/>
-    <row r="622" ht="15.75" customHeight="1"/>
-    <row r="623" ht="15.75" customHeight="1"/>
-    <row r="624" ht="15.75" customHeight="1"/>
-    <row r="625" ht="15.75" customHeight="1"/>
-    <row r="626" ht="15.75" customHeight="1"/>
-    <row r="627" ht="15.75" customHeight="1"/>
-    <row r="628" ht="15.75" customHeight="1"/>
-    <row r="629" ht="15.75" customHeight="1"/>
-    <row r="630" ht="15.75" customHeight="1"/>
-    <row r="631" ht="15.75" customHeight="1"/>
-    <row r="632" ht="15.75" customHeight="1"/>
-    <row r="633" ht="15.75" customHeight="1"/>
-    <row r="634" ht="15.75" customHeight="1"/>
-    <row r="635" ht="15.75" customHeight="1"/>
-    <row r="636" ht="15.75" customHeight="1"/>
-    <row r="637" ht="15.75" customHeight="1"/>
-    <row r="638" ht="15.75" customHeight="1"/>
-    <row r="639" ht="15.75" customHeight="1"/>
-    <row r="640" ht="15.75" customHeight="1"/>
-    <row r="641" ht="15.75" customHeight="1"/>
-    <row r="642" ht="15.75" customHeight="1"/>
-    <row r="643" ht="15.75" customHeight="1"/>
-    <row r="644" ht="15.75" customHeight="1"/>
-    <row r="645" ht="15.75" customHeight="1"/>
-    <row r="646" ht="15.75" customHeight="1"/>
-    <row r="647" ht="15.75" customHeight="1"/>
-    <row r="648" ht="15.75" customHeight="1"/>
-    <row r="649" ht="15.75" customHeight="1"/>
-    <row r="650" ht="15.75" customHeight="1"/>
-    <row r="651" ht="15.75" customHeight="1"/>
-    <row r="652" ht="15.75" customHeight="1"/>
-    <row r="653" ht="15.75" customHeight="1"/>
-    <row r="654" ht="15.75" customHeight="1"/>
-    <row r="655" ht="15.75" customHeight="1"/>
-    <row r="656" ht="15.75" customHeight="1"/>
-    <row r="657" ht="15.75" customHeight="1"/>
-    <row r="658" ht="15.75" customHeight="1"/>
-    <row r="659" ht="15.75" customHeight="1"/>
-    <row r="660" ht="15.75" customHeight="1"/>
-    <row r="661" ht="15.75" customHeight="1"/>
-    <row r="662" ht="15.75" customHeight="1"/>
-    <row r="663" ht="15.75" customHeight="1"/>
-    <row r="664" ht="15.75" customHeight="1"/>
-    <row r="665" ht="15.75" customHeight="1"/>
-    <row r="666" ht="15.75" customHeight="1"/>
-    <row r="667" ht="15.75" customHeight="1"/>
-    <row r="668" ht="15.75" customHeight="1"/>
-    <row r="669" ht="15.75" customHeight="1"/>
-    <row r="670" ht="15.75" customHeight="1"/>
-    <row r="671" ht="15.75" customHeight="1"/>
-    <row r="672" ht="15.75" customHeight="1"/>
-    <row r="673" ht="15.75" customHeight="1"/>
-    <row r="674" ht="15.75" customHeight="1"/>
-    <row r="675" ht="15.75" customHeight="1"/>
-    <row r="676" ht="15.75" customHeight="1"/>
-    <row r="677" ht="15.75" customHeight="1"/>
-    <row r="678" ht="15.75" customHeight="1"/>
-    <row r="679" ht="15.75" customHeight="1"/>
-    <row r="680" ht="15.75" customHeight="1"/>
-    <row r="681" ht="15.75" customHeight="1"/>
-    <row r="682" ht="15.75" customHeight="1"/>
-    <row r="683" ht="15.75" customHeight="1"/>
-    <row r="684" ht="15.75" customHeight="1"/>
-    <row r="685" ht="15.75" customHeight="1"/>
-    <row r="686" ht="15.75" customHeight="1"/>
-    <row r="687" ht="15.75" customHeight="1"/>
-    <row r="688" ht="15.75" customHeight="1"/>
-    <row r="689" ht="15.75" customHeight="1"/>
-    <row r="690" ht="15.75" customHeight="1"/>
-    <row r="691" ht="15.75" customHeight="1"/>
-    <row r="692" ht="15.75" customHeight="1"/>
-    <row r="693" ht="15.75" customHeight="1"/>
-    <row r="694" ht="15.75" customHeight="1"/>
-    <row r="695" ht="15.75" customHeight="1"/>
-    <row r="696" ht="15.75" customHeight="1"/>
-    <row r="697" ht="15.75" customHeight="1"/>
-    <row r="698" ht="15.75" customHeight="1"/>
-    <row r="699" ht="15.75" customHeight="1"/>
-    <row r="700" ht="15.75" customHeight="1"/>
-    <row r="701" ht="15.75" customHeight="1"/>
-    <row r="702" ht="15.75" customHeight="1"/>
-    <row r="703" ht="15.75" customHeight="1"/>
-    <row r="704" ht="15.75" customHeight="1"/>
-    <row r="705" ht="15.75" customHeight="1"/>
-    <row r="706" ht="15.75" customHeight="1"/>
-    <row r="707" ht="15.75" customHeight="1"/>
-    <row r="708" ht="15.75" customHeight="1"/>
-    <row r="709" ht="15.75" customHeight="1"/>
-    <row r="710" ht="15.75" customHeight="1"/>
-    <row r="711" ht="15.75" customHeight="1"/>
-    <row r="712" ht="15.75" customHeight="1"/>
-    <row r="713" ht="15.75" customHeight="1"/>
-    <row r="714" ht="15.75" customHeight="1"/>
-    <row r="715" ht="15.75" customHeight="1"/>
-    <row r="716" ht="15.75" customHeight="1"/>
-    <row r="717" ht="15.75" customHeight="1"/>
-    <row r="718" ht="15.75" customHeight="1"/>
-    <row r="719" ht="15.75" customHeight="1"/>
-    <row r="720" ht="15.75" customHeight="1"/>
-    <row r="721" ht="15.75" customHeight="1"/>
-    <row r="722" ht="15.75" customHeight="1"/>
-    <row r="723" ht="15.75" customHeight="1"/>
-    <row r="724" ht="15.75" customHeight="1"/>
-    <row r="725" ht="15.75" customHeight="1"/>
-    <row r="726" ht="15.75" customHeight="1"/>
-    <row r="727" ht="15.75" customHeight="1"/>
-    <row r="728" ht="15.75" customHeight="1"/>
-    <row r="729" ht="15.75" customHeight="1"/>
-    <row r="730" ht="15.75" customHeight="1"/>
-    <row r="731" ht="15.75" customHeight="1"/>
-    <row r="732" ht="15.75" customHeight="1"/>
-    <row r="733" ht="15.75" customHeight="1"/>
-    <row r="734" ht="15.75" customHeight="1"/>
-    <row r="735" ht="15.75" customHeight="1"/>
-    <row r="736" ht="15.75" customHeight="1"/>
-    <row r="737" ht="15.75" customHeight="1"/>
-    <row r="738" ht="15.75" customHeight="1"/>
-    <row r="739" ht="15.75" customHeight="1"/>
-    <row r="740" ht="15.75" customHeight="1"/>
-    <row r="741" ht="15.75" customHeight="1"/>
-    <row r="742" ht="15.75" customHeight="1"/>
-    <row r="743" ht="15.75" customHeight="1"/>
-    <row r="744" ht="15.75" customHeight="1"/>
-    <row r="745" ht="15.75" customHeight="1"/>
-    <row r="746" ht="15.75" customHeight="1"/>
-    <row r="747" ht="15.75" customHeight="1"/>
-    <row r="748" ht="15.75" customHeight="1"/>
-    <row r="749" ht="15.75" customHeight="1"/>
-    <row r="750" ht="15.75" customHeight="1"/>
-    <row r="751" ht="15.75" customHeight="1"/>
-    <row r="752" ht="15.75" customHeight="1"/>
-    <row r="753" ht="15.75" customHeight="1"/>
-    <row r="754" ht="15.75" customHeight="1"/>
-    <row r="755" ht="15.75" customHeight="1"/>
-    <row r="756" ht="15.75" customHeight="1"/>
-    <row r="757" ht="15.75" customHeight="1"/>
-    <row r="758" ht="15.75" customHeight="1"/>
-    <row r="759" ht="15.75" customHeight="1"/>
-    <row r="760" ht="15.75" customHeight="1"/>
-    <row r="761" ht="15.75" customHeight="1"/>
-    <row r="762" ht="15.75" customHeight="1"/>
-    <row r="763" ht="15.75" customHeight="1"/>
-    <row r="764" ht="15.75" customHeight="1"/>
-    <row r="765" ht="15.75" customHeight="1"/>
-    <row r="766" ht="15.75" customHeight="1"/>
-    <row r="767" ht="15.75" customHeight="1"/>
-    <row r="768" ht="15.75" customHeight="1"/>
-    <row r="769" ht="15.75" customHeight="1"/>
-    <row r="770" ht="15.75" customHeight="1"/>
-    <row r="771" ht="15.75" customHeight="1"/>
-    <row r="772" ht="15.75" customHeight="1"/>
-    <row r="773" ht="15.75" customHeight="1"/>
-    <row r="774" ht="15.75" customHeight="1"/>
-    <row r="775" ht="15.75" customHeight="1"/>
-    <row r="776" ht="15.75" customHeight="1"/>
-    <row r="777" ht="15.75" customHeight="1"/>
-    <row r="778" ht="15.75" customHeight="1"/>
-    <row r="779" ht="15.75" customHeight="1"/>
-    <row r="780" ht="15.75" customHeight="1"/>
-    <row r="781" ht="15.75" customHeight="1"/>
-    <row r="782" ht="15.75" customHeight="1"/>
-    <row r="783" ht="15.75" customHeight="1"/>
-    <row r="784" ht="15.75" customHeight="1"/>
-    <row r="785" ht="15.75" customHeight="1"/>
-    <row r="786" ht="15.75" customHeight="1"/>
-    <row r="787" ht="15.75" customHeight="1"/>
-    <row r="788" ht="15.75" customHeight="1"/>
-    <row r="789" ht="15.75" customHeight="1"/>
-    <row r="790" ht="15.75" customHeight="1"/>
-    <row r="791" ht="15.75" customHeight="1"/>
-    <row r="792" ht="15.75" customHeight="1"/>
-    <row r="793" ht="15.75" customHeight="1"/>
-    <row r="794" ht="15.75" customHeight="1"/>
-    <row r="795" ht="15.75" customHeight="1"/>
-    <row r="796" ht="15.75" customHeight="1"/>
-    <row r="797" ht="15.75" customHeight="1"/>
-    <row r="798" ht="15.75" customHeight="1"/>
-    <row r="799" ht="15.75" customHeight="1"/>
-    <row r="800" ht="15.75" customHeight="1"/>
-    <row r="801" ht="15.75" customHeight="1"/>
-    <row r="802" ht="15.75" customHeight="1"/>
-    <row r="803" ht="15.75" customHeight="1"/>
-    <row r="804" ht="15.75" customHeight="1"/>
-    <row r="805" ht="15.75" customHeight="1"/>
-    <row r="806" ht="15.75" customHeight="1"/>
-    <row r="807" ht="15.75" customHeight="1"/>
-    <row r="808" ht="15.75" customHeight="1"/>
-    <row r="809" ht="15.75" customHeight="1"/>
-    <row r="810" ht="15.75" customHeight="1"/>
-    <row r="811" ht="15.75" customHeight="1"/>
-    <row r="812" ht="15.75" customHeight="1"/>
-    <row r="813" ht="15.75" customHeight="1"/>
-    <row r="814" ht="15.75" customHeight="1"/>
-    <row r="815" ht="15.75" customHeight="1"/>
-    <row r="816" ht="15.75" customHeight="1"/>
-    <row r="817" ht="15.75" customHeight="1"/>
-    <row r="818" ht="15.75" customHeight="1"/>
-    <row r="819" ht="15.75" customHeight="1"/>
-    <row r="820" ht="15.75" customHeight="1"/>
-    <row r="821" ht="15.75" customHeight="1"/>
-    <row r="822" ht="15.75" customHeight="1"/>
-    <row r="823" ht="15.75" customHeight="1"/>
-    <row r="824" ht="15.75" customHeight="1"/>
-    <row r="825" ht="15.75" customHeight="1"/>
-    <row r="826" ht="15.75" customHeight="1"/>
-    <row r="827" ht="15.75" customHeight="1"/>
-    <row r="828" ht="15.75" customHeight="1"/>
-    <row r="829" ht="15.75" customHeight="1"/>
-    <row r="830" ht="15.75" customHeight="1"/>
-    <row r="831" ht="15.75" customHeight="1"/>
-    <row r="832" ht="15.75" customHeight="1"/>
-    <row r="833" ht="15.75" customHeight="1"/>
-    <row r="834" ht="15.75" customHeight="1"/>
-    <row r="835" ht="15.75" customHeight="1"/>
-    <row r="836" ht="15.75" customHeight="1"/>
-    <row r="837" ht="15.75" customHeight="1"/>
-    <row r="838" ht="15.75" customHeight="1"/>
-    <row r="839" ht="15.75" customHeight="1"/>
-    <row r="840" ht="15.75" customHeight="1"/>
-    <row r="841" ht="15.75" customHeight="1"/>
-    <row r="842" ht="15.75" customHeight="1"/>
-    <row r="843" ht="15.75" customHeight="1"/>
-    <row r="844" ht="15.75" customHeight="1"/>
-    <row r="845" ht="15.75" customHeight="1"/>
-    <row r="846" ht="15.75" customHeight="1"/>
-    <row r="847" ht="15.75" customHeight="1"/>
-    <row r="848" ht="15.75" customHeight="1"/>
-    <row r="849" ht="15.75" customHeight="1"/>
-    <row r="850" ht="15.75" customHeight="1"/>
-    <row r="851" ht="15.75" customHeight="1"/>
-    <row r="852" ht="15.75" customHeight="1"/>
-    <row r="853" ht="15.75" customHeight="1"/>
-    <row r="854" ht="15.75" customHeight="1"/>
-    <row r="855" ht="15.75" customHeight="1"/>
-    <row r="856" ht="15.75" customHeight="1"/>
-    <row r="857" ht="15.75" customHeight="1"/>
-    <row r="858" ht="15.75" customHeight="1"/>
-    <row r="859" ht="15.75" customHeight="1"/>
-    <row r="860" ht="15.75" customHeight="1"/>
-    <row r="861" ht="15.75" customHeight="1"/>
-    <row r="862" ht="15.75" customHeight="1"/>
-    <row r="863" ht="15.75" customHeight="1"/>
-    <row r="864" ht="15.75" customHeight="1"/>
-    <row r="865" ht="15.75" customHeight="1"/>
-    <row r="866" ht="15.75" customHeight="1"/>
-    <row r="867" ht="15.75" customHeight="1"/>
-    <row r="868" ht="15.75" customHeight="1"/>
-    <row r="869" ht="15.75" customHeight="1"/>
-    <row r="870" ht="15.75" customHeight="1"/>
-    <row r="871" ht="15.75" customHeight="1"/>
-    <row r="872" ht="15.75" customHeight="1"/>
-    <row r="873" ht="15.75" customHeight="1"/>
-    <row r="874" ht="15.75" customHeight="1"/>
-    <row r="875" ht="15.75" customHeight="1"/>
-    <row r="876" ht="15.75" customHeight="1"/>
-    <row r="877" ht="15.75" customHeight="1"/>
-    <row r="878" ht="15.75" customHeight="1"/>
-    <row r="879" ht="15.75" customHeight="1"/>
-    <row r="880" ht="15.75" customHeight="1"/>
-    <row r="881" ht="15.75" customHeight="1"/>
-    <row r="882" ht="15.75" customHeight="1"/>
-    <row r="883" ht="15.75" customHeight="1"/>
-    <row r="884" ht="15.75" customHeight="1"/>
-    <row r="885" ht="15.75" customHeight="1"/>
-    <row r="886" ht="15.75" customHeight="1"/>
-    <row r="887" ht="15.75" customHeight="1"/>
-    <row r="888" ht="15.75" customHeight="1"/>
-    <row r="889" ht="15.75" customHeight="1"/>
-    <row r="890" ht="15.75" customHeight="1"/>
-    <row r="891" ht="15.75" customHeight="1"/>
-    <row r="892" ht="15.75" customHeight="1"/>
-    <row r="893" ht="15.75" customHeight="1"/>
-    <row r="894" ht="15.75" customHeight="1"/>
-    <row r="895" ht="15.75" customHeight="1"/>
-    <row r="896" ht="15.75" customHeight="1"/>
-    <row r="897" ht="15.75" customHeight="1"/>
-    <row r="898" ht="15.75" customHeight="1"/>
-    <row r="899" ht="15.75" customHeight="1"/>
-    <row r="900" ht="15.75" customHeight="1"/>
-    <row r="901" ht="15.75" customHeight="1"/>
-    <row r="902" ht="15.75" customHeight="1"/>
-    <row r="903" ht="15.75" customHeight="1"/>
-    <row r="904" ht="15.75" customHeight="1"/>
-    <row r="905" ht="15.75" customHeight="1"/>
-    <row r="906" ht="15.75" customHeight="1"/>
-    <row r="907" ht="15.75" customHeight="1"/>
-    <row r="908" ht="15.75" customHeight="1"/>
-    <row r="909" ht="15.75" customHeight="1"/>
-    <row r="910" ht="15.75" customHeight="1"/>
-    <row r="911" ht="15.75" customHeight="1"/>
-    <row r="912" ht="15.75" customHeight="1"/>
-    <row r="913" ht="15.75" customHeight="1"/>
-    <row r="914" ht="15.75" customHeight="1"/>
-    <row r="915" ht="15.75" customHeight="1"/>
-    <row r="916" ht="15.75" customHeight="1"/>
-    <row r="917" ht="15.75" customHeight="1"/>
-    <row r="918" ht="15.75" customHeight="1"/>
-    <row r="919" ht="15.75" customHeight="1"/>
-    <row r="920" ht="15.75" customHeight="1"/>
-    <row r="921" ht="15.75" customHeight="1"/>
-    <row r="922" ht="15.75" customHeight="1"/>
-    <row r="923" ht="15.75" customHeight="1"/>
-    <row r="924" ht="15.75" customHeight="1"/>
-    <row r="925" ht="15.75" customHeight="1"/>
-    <row r="926" ht="15.75" customHeight="1"/>
-    <row r="927" ht="15.75" customHeight="1"/>
-    <row r="928" ht="15.75" customHeight="1"/>
-    <row r="929" ht="15.75" customHeight="1"/>
-    <row r="930" ht="15.75" customHeight="1"/>
-    <row r="931" ht="15.75" customHeight="1"/>
-    <row r="932" ht="15.75" customHeight="1"/>
-    <row r="933" ht="15.75" customHeight="1"/>
-    <row r="934" ht="15.75" customHeight="1"/>
-    <row r="935" ht="15.75" customHeight="1"/>
-    <row r="936" ht="15.75" customHeight="1"/>
-    <row r="937" ht="15.75" customHeight="1"/>
-    <row r="938" ht="15.75" customHeight="1"/>
-    <row r="939" ht="15.75" customHeight="1"/>
-    <row r="940" ht="15.75" customHeight="1"/>
-    <row r="941" ht="15.75" customHeight="1"/>
-    <row r="942" ht="15.75" customHeight="1"/>
-    <row r="943" ht="15.75" customHeight="1"/>
-    <row r="944" ht="15.75" customHeight="1"/>
-    <row r="945" ht="15.75" customHeight="1"/>
-    <row r="946" ht="15.75" customHeight="1"/>
-    <row r="947" ht="15.75" customHeight="1"/>
-    <row r="948" ht="15.75" customHeight="1"/>
-    <row r="949" ht="15.75" customHeight="1"/>
-    <row r="950" ht="15.75" customHeight="1"/>
-    <row r="951" ht="15.75" customHeight="1"/>
-    <row r="952" ht="15.75" customHeight="1"/>
-    <row r="953" ht="15.75" customHeight="1"/>
-    <row r="954" ht="15.75" customHeight="1"/>
-    <row r="955" ht="15.75" customHeight="1"/>
-    <row r="956" ht="15.75" customHeight="1"/>
-    <row r="957" ht="15.75" customHeight="1"/>
-    <row r="958" ht="15.75" customHeight="1"/>
-    <row r="959" ht="15.75" customHeight="1"/>
-    <row r="960" ht="15.75" customHeight="1"/>
-    <row r="961" ht="15.75" customHeight="1"/>
-    <row r="962" ht="15.75" customHeight="1"/>
-    <row r="963" ht="15.75" customHeight="1"/>
-    <row r="964" ht="15.75" customHeight="1"/>
-    <row r="965" ht="15.75" customHeight="1"/>
-    <row r="966" ht="15.75" customHeight="1"/>
-    <row r="967" ht="15.75" customHeight="1"/>
-    <row r="968" ht="15.75" customHeight="1"/>
-    <row r="969" ht="15.75" customHeight="1"/>
-    <row r="970" ht="15.75" customHeight="1"/>
-    <row r="971" ht="15.75" customHeight="1"/>
-    <row r="972" ht="15.75" customHeight="1"/>
-    <row r="973" ht="15.75" customHeight="1"/>
-    <row r="974" ht="15.75" customHeight="1"/>
-    <row r="975" ht="15.75" customHeight="1"/>
-    <row r="976" ht="15.75" customHeight="1"/>
-    <row r="977" ht="15.75" customHeight="1"/>
-    <row r="978" ht="15.75" customHeight="1"/>
-    <row r="979" ht="15.75" customHeight="1"/>
-    <row r="980" ht="15.75" customHeight="1"/>
-    <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
-    <row r="985" ht="15.75" customHeight="1"/>
-    <row r="986" ht="15.75" customHeight="1"/>
-    <row r="987" ht="15.75" customHeight="1"/>
-    <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="229" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="230" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="231" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="232" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="233" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="234" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="235" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="236" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="237" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="238" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="239" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="240" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>